<commit_message>
Removed trailing blank in name of 2nd column in the historical_items.[xlsx,csv] files: 'text ' ==> 'text'.
</commit_message>
<xml_diff>
--- a/xlsx/historical_items.xlsx
+++ b/xlsx/historical_items.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Desktop\ken_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C97BCD8-D5F8-45AC-9FD6-C39E8574F4BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2F564D-1303-46F6-87E0-28DBB18C4F4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{171EF181-1F3C-7A42-9B63-D835B687641B}"/>
   </bookViews>
@@ -501,7 +501,7 @@
     <t>year</t>
   </si>
   <si>
-    <t xml:space="preserve">text </t>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -887,9 +887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8479D0E-E3F6-DA41-AEC9-2CE4981D9A6E}">
   <dimension ref="A1:B160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
New historical data spreadsheet from Ken 3/8/21 - known NOT to be final.
</commit_message>
<xml_diff>
--- a/xlsx/historical_items.xlsx
+++ b/xlsx/historical_items.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2F564D-1303-46F6-87E0-28DBB18C4F4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAF0541-4287-4D34-8DFA-EF247C4F9EB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{171EF181-1F3C-7A42-9B63-D835B687641B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="366">
   <si>
     <t>The U.S. capital is moved from Philadelphia to Washington, DC.</t>
   </si>
@@ -57,12 +57,6 @@
     <t>Robert Fulton patents steamboat.</t>
   </si>
   <si>
-    <t>Allardyce Barclay begins a bet of walking 1 mile every hour for 1,000 hours. Each hour he walked a mile round trip from his home.</t>
-  </si>
-  <si>
-    <t>1st US steamboat to a make an ocean voyage leaves NY for Philadelphia.</t>
-  </si>
-  <si>
     <t>The first steam-powered ferry service between New York City and Hoboken, New Jersey.</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>First commercially successful self-propelled engine on land was Mathew Murray's Salamanca on Middleton Railway using toothed wheels and rail.</t>
   </si>
   <si>
-    <t>1st US raw cotton-to-cloth mill founded in Waltham, Massachusetts.</t>
-  </si>
-  <si>
     <t>"Star Spangled Banner" published as a song, lyrics by Francis Scott Key, tune by John Stafford Smith.</t>
   </si>
   <si>
@@ -93,12 +84,6 @@
     <t>Denis Johnson invents kick scooter.</t>
   </si>
   <si>
-    <t>1st bicycles (swift walkers) in US introduced in NYC.</t>
-  </si>
-  <si>
-    <t>1st ship sails through the Erie Canal from Rome, New York to Utica, New York.</t>
-  </si>
-  <si>
     <t>Antarctica sighted by US Navy Captain Nathaniel B. Palmer.</t>
   </si>
   <si>
@@ -108,12 +93,6 @@
     <t>First ground is broken at Allenburg for the building of the original Welland Canal, Ontario, Canada.</t>
   </si>
   <si>
-    <t>George Stephenson's "Locomotion No. 1" becomes the 1st steam locomotive to carry passengers on a public rail line, the Stockton and Darlington Railway in England.</t>
-  </si>
-  <si>
-    <t>1st steamboat to navigate the Mississippi River arrives at Fort Snelling.</t>
-  </si>
-  <si>
     <t>James Weddell reaches the South Pole.</t>
   </si>
   <si>
@@ -123,12 +102,6 @@
     <t>The Menai Suspension Bridge, considered the world's first modern suspension bridge, connecting the Isle of Anglesey to the north West coast of Wales is opened.</t>
   </si>
   <si>
-    <t>1st commercial railroad in US, Baltimore &amp; Ohio (B&amp;O) chartered</t>
-  </si>
-  <si>
-    <t>1st US swimming school opens (Boston, Massachusetts).</t>
-  </si>
-  <si>
     <t>Bolton and Leigh Railway opens to freight traffic.</t>
   </si>
   <si>
@@ -138,42 +111,18 @@
     <t>Delaware River &amp; Chesapeake Bay Canal formally opens.</t>
   </si>
   <si>
-    <t>1st stone arch railroad bridge in US dedicated, Baltimore.</t>
-  </si>
-  <si>
-    <t>1st US Railroad Station opens (Baltimore).</t>
-  </si>
-  <si>
-    <t>1st railroad timetable published in newspaper (Baltimore American).</t>
-  </si>
-  <si>
     <t>First passenger to be killed by a railway train (William Huskisson, England).</t>
   </si>
   <si>
     <t>Oliver Wendell Holmes writes poem "Old Ironsides" as tribute to the 18th-century USS Constitution.</t>
   </si>
   <si>
-    <t>1st practical US coal-burning locomotive makes 1st trial run in Pennsylvania.</t>
-  </si>
-  <si>
     <t>London Bridge opens to traffic.</t>
   </si>
   <si>
     <t>Erie Canal closes for entire month due to cold weather.</t>
   </si>
   <si>
-    <t>1st railroad accident in US, Granite Railway, Quincy, Massachusetts, kills 1.</t>
-  </si>
-  <si>
-    <t>1st streetcar railway in America starts operating in New York City with 12 cent fare.</t>
-  </si>
-  <si>
-    <t>Boston Academy of Music, 1st US music school, established.</t>
-  </si>
-  <si>
-    <t>1st railroad tunnel in US completed, in Pennsylvania.</t>
-  </si>
-  <si>
     <t>St Etienne-Lyons railway opens in France.</t>
   </si>
   <si>
@@ -189,9 +138,6 @@
     <t>The first electric locomotive built in 1837 was a battery locomotive. It was built by chemist Robert Davidson of Aberdeen in Scotland, and it was powered by galvanic cells (batteries).</t>
   </si>
   <si>
-    <t>Euston railway station opens in London as the terminus of the London and Birmingham Railway (L&amp;BR), the city's 1st intercity railway station.</t>
-  </si>
-  <si>
     <t>Steam shovel patented by William Otis, Philadelphia.</t>
   </si>
   <si>
@@ -213,9 +159,6 @@
     <t>Isambard Kingdom Brunel's SS Great Western, the first purpose-built transatlantic steamship, inaugurates the first regular transatlantic steamship service.</t>
   </si>
   <si>
-    <t>1st US wire suspension bridge for general traffic opens in Pennsylvania.</t>
-  </si>
-  <si>
     <t>The first wagon train to California, with sixty-nine adults and several children, leave from Independence, Missouri.</t>
   </si>
   <si>
@@ -243,9 +186,6 @@
     <t>New Haven Railroad opens.</t>
   </si>
   <si>
-    <t>1st passenger train service to Peekskill, New York (New Haven Railroad).</t>
-  </si>
-  <si>
     <t>California becomes 31th state of the Union.</t>
   </si>
   <si>
@@ -258,45 +198,21 @@
     <t>Elisha Otis invents the safety elevator.</t>
   </si>
   <si>
-    <t>Completion of Grand Trunk Line, trains begin running over 1st North American railroad between Portland, Maine and Montreal</t>
-  </si>
-  <si>
-    <t>1st round-the-world trip by yacht (Cornelius Vanderbilt).</t>
-  </si>
-  <si>
     <t>The first bridge over the Mississippi River opens in what is now Minneapolis, Minnesota.</t>
   </si>
   <si>
-    <t>1st train crosses 1st US railway suspension bridge, Niagara Falls.</t>
-  </si>
-  <si>
-    <t>1st train crosses Mississippi River's 1st bridge, from Rock Island, Illinois to Davenport, Iowa.</t>
-  </si>
-  <si>
-    <t>1st park land purchased by a US city, Worcester, Massachusetts.</t>
-  </si>
-  <si>
-    <t>Georgia becomes 1st state to regulate railroads.</t>
-  </si>
-  <si>
     <t>The first elevator is installed by Elisha Otis on Broadway in New York City.</t>
   </si>
   <si>
     <t>The first transatlantic cable is completed.</t>
   </si>
   <si>
-    <t>Streetcar patented (E A Gardner of Philadelphia).</t>
-  </si>
-  <si>
     <t>Minnesota becomes 32th state of the Union.</t>
   </si>
   <si>
     <t>Oregon becomes 33th state of the Union.</t>
   </si>
   <si>
-    <t>1st Pullman sleeping car in service.</t>
-  </si>
-  <si>
     <t>Gaston Planté invented the lead–acid rechargeable battery</t>
   </si>
   <si>
@@ -309,42 +225,21 @@
     <t>Steam elevator patented by Elisha Otis.</t>
   </si>
   <si>
-    <t>1st underground railway opens in London.</t>
-  </si>
-  <si>
     <t>West Virginia becomes 35th state of the Union.</t>
   </si>
   <si>
     <t>Nevada becomes 36th state of the Union.</t>
   </si>
   <si>
-    <t>The first narrow gauge mainline railway in the world opens at Grandchester, Australia.</t>
-  </si>
-  <si>
-    <t>Work begins on 1st US underwater highway tunnel in Chicago.</t>
-  </si>
-  <si>
     <t>Nebraska becomes 37th state of the Union.</t>
   </si>
   <si>
-    <t>1st US elevated railroad begins service, NYC.</t>
-  </si>
-  <si>
     <t>The first traffic lights are installed outside the Palace of Westminster in London.</t>
   </si>
   <si>
     <t>Boston University is chartered by the Commonwealth of Massachusetts</t>
   </si>
   <si>
-    <t>Golden Spike driven, completing the 1st US Transcontinental Railroad at Promontory Summit, Utah and connecting the Central Pacific Railroad with the Union Pacific.</t>
-  </si>
-  <si>
-    <t>1st trans-US rail service begins.</t>
-  </si>
-  <si>
-    <t>1st cable car patented, by Andrew Smith Hallidie in the US.</t>
-  </si>
-  <si>
     <t>US engineer George Brayton patents an internal combustion engine.</t>
   </si>
   <si>
@@ -354,9 +249,6 @@
     <t>Regular Cable Car service begins on Clay Street, San Francisco.</t>
   </si>
   <si>
-    <t>1st recorded dam disaster in US (Williamsburg, Massachusetts).</t>
-  </si>
-  <si>
     <t>World's first electric tram line operated in Sestroretsk near Saint Petersburg, Russia.</t>
   </si>
   <si>
@@ -366,21 +258,9 @@
     <t>An express train called the Transcontinental Express arrives in San Francisco, California, via the First Transcontinental Railroad only 83 hours and 39 minutes after having left New York City.</t>
   </si>
   <si>
-    <t>1st cantilever bridge in US completed, Harrodsburg, Kentucky.</t>
-  </si>
-  <si>
-    <t>1st female telephone operator starts work (Emma Nutt in Boston).</t>
-  </si>
-  <si>
-    <t>1st mobile home (horse drawn) used in a journey from London &amp; Cyprus.</t>
-  </si>
-  <si>
     <t>The construction of the Panama Canal begins.</t>
   </si>
   <si>
-    <t>World's 1st electric tram enters service in Lichterfelder (near Berlin).</t>
-  </si>
-  <si>
     <t>The "Elektromote" - forerunner of the trolleybus - is tested by Werner von Siemens in Berlin.</t>
   </si>
   <si>
@@ -393,9 +273,6 @@
     <t>The railroads of the Southern United States convert 11,000 miles of track from a five foot rail gauge to standard gauge.</t>
   </si>
   <si>
-    <t>Thomas Stevens is 1st man to bicycle around the world (San Francisco to San Francisco).</t>
-  </si>
-  <si>
     <t>Scottish vet John Boyd Dunlop patents pneumatic bicycle tyre.</t>
   </si>
   <si>
@@ -420,18 +297,12 @@
     <t>Electric self-starter for automobile patented.</t>
   </si>
   <si>
-    <t>San Francisco Bay City Club opens 1st US bicycle race track, made of wood.</t>
-  </si>
-  <si>
     <t>Hildebrand &amp; Wolfmüller became the first motorcycle available to the public for purchase.</t>
   </si>
   <si>
     <t>Charles Duryea patents a gas-driven automobile.</t>
   </si>
   <si>
-    <t>America's 1st auto race organised in Chicago, Frank Duryea wins averaging 7 MPH.</t>
-  </si>
-  <si>
     <t>Utah becomes 45th state of the Union.</t>
   </si>
   <si>
@@ -496,6 +367,756 @@
   </si>
   <si>
     <t>Alessandro Volta invinted the electric battery.</t>
+  </si>
+  <si>
+    <t>The first Boston Marathon is run with fifteen runners, won by John McDermott.</t>
+  </si>
+  <si>
+    <t>The era of the subway begins when the first underground public transportation in North America opens in Boston, Massachusetts.</t>
+  </si>
+  <si>
+    <t>Winton Motor Carriage Company publishes the first known automobile ad in Scientific American using the headline “dispense with a horse.”</t>
+  </si>
+  <si>
+    <t>Rudolf Diesel of Germany obtains patent for his internal combustion engine, later known as the diesel engine</t>
+  </si>
+  <si>
+    <t>Ferdinand von Zeppelin builds the first successful airship.</t>
+  </si>
+  <si>
+    <t>New York City breaks ground for a new underground "Rapid Transit Railroad" that would link Manhattan and Brooklyn.</t>
+  </si>
+  <si>
+    <t>World's longest railroad tunnel (Simplon) linking Italy and Switzerland opens.</t>
+  </si>
+  <si>
+    <t>Santos-Dumont proves airship manoeuverable by circling Eiffel Tower.</t>
+  </si>
+  <si>
+    <t>American Automobile Association (AAA) founded in Chicago.</t>
+  </si>
+  <si>
+    <t>Orville Wright and Wilbur Wright – Fly the first motor-driven airplane.</t>
+  </si>
+  <si>
+    <t>New bicycle race "Tour de France" announced.</t>
+  </si>
+  <si>
+    <t>The first non-experimental trolleybus system was a seasonal municipal line installed near Nantasket Beach, Hull, Massachusetts.</t>
+  </si>
+  <si>
+    <t>After 13 years, the 4,607-mile Trans-Siberian railway is completed.</t>
+  </si>
+  <si>
+    <t>First section of New York subway - Lower Manhattan to Broadway Harlem, opened by Interborough Rapid Transit (IRT), fare one nickel.</t>
+  </si>
+  <si>
+    <t>Early hydrofoil used by Enrico Forlanini.</t>
+  </si>
+  <si>
+    <t>Oklahoma becomes 46th state of the Union.</t>
+  </si>
+  <si>
+    <t>Taxis begin running in NYC.</t>
+  </si>
+  <si>
+    <t>First US steamboat to a make an ocean voyage leaves NY for Philadelphia.</t>
+  </si>
+  <si>
+    <t>First US raw cotton-to-cloth mill founded in Waltham, Massachusetts.</t>
+  </si>
+  <si>
+    <t>First bicycles (swift walkers) in US introduced in NYC.</t>
+  </si>
+  <si>
+    <t>First ship sails through the Erie Canal from Rome, New York to Utica, New York.</t>
+  </si>
+  <si>
+    <t>First steamboat to navigate the Mississippi River arrives at Fort Snelling.</t>
+  </si>
+  <si>
+    <t>George Stephenson's "Locomotion No. 1" becomes the First steam locomotive to carry passengers on a public rail line, the Stockton and Darlington Railway in England.</t>
+  </si>
+  <si>
+    <t>First commercial railroad in US, Baltimore &amp; Ohio (B&amp;O) chartered</t>
+  </si>
+  <si>
+    <t>First US swimming school opens (Boston, Massachusetts).</t>
+  </si>
+  <si>
+    <t>First stone arch railroad bridge in US dedicated, Baltimore.</t>
+  </si>
+  <si>
+    <t>First US Railroad Station opens (Baltimore).</t>
+  </si>
+  <si>
+    <t>First railroad timetable published in newspaper (Baltimore American).</t>
+  </si>
+  <si>
+    <t>First practical US coal-burning locomotive makes First trial run in Pennsylvania.</t>
+  </si>
+  <si>
+    <t>First streetcar railway in America starts operating in New York City with 12 cent fare.</t>
+  </si>
+  <si>
+    <t>Boston Academy of Music, First US music school, established.</t>
+  </si>
+  <si>
+    <t>First railroad tunnel in US completed, in Pennsylvania.</t>
+  </si>
+  <si>
+    <t>Euston railway station opens in London as the terminus of the London and Birmingham Railway (L&amp;BR), the city's First intercity railway station.</t>
+  </si>
+  <si>
+    <t>First US wire suspension bridge for general traffic opens in Pennsylvania.</t>
+  </si>
+  <si>
+    <t>First passenger train service to Peekskill, New York (New Haven Railroad).</t>
+  </si>
+  <si>
+    <t>Completion of Grand Trunk Line, trains begin running over First North American railroad between Portland, Maine and Montreal</t>
+  </si>
+  <si>
+    <t>First round-the-world trip by yacht (Cornelius Vanderbilt).</t>
+  </si>
+  <si>
+    <t>First park land purchased by a US city, Worcester, Massachusetts.</t>
+  </si>
+  <si>
+    <t>First train crosses First US railway suspension bridge, Niagara Falls.</t>
+  </si>
+  <si>
+    <t>First train crosses Mississippi River's First bridge, from Rock Island, Illinois to Davenport, Iowa.</t>
+  </si>
+  <si>
+    <t>Georgia becomes First state to regulate railroads.</t>
+  </si>
+  <si>
+    <t>First Pullman sleeping car in service.</t>
+  </si>
+  <si>
+    <t>First underground railway opens in London.</t>
+  </si>
+  <si>
+    <t>Work begins on First US underwater highway tunnel in Chicago.</t>
+  </si>
+  <si>
+    <t>First US elevated railroad begins service, NYC.</t>
+  </si>
+  <si>
+    <t>Golden Spike driven, completing the First US Transcontinental Railroad at Promontory Summit, Utah and connecting the Central Pacific Railroad with the Union Pacific.</t>
+  </si>
+  <si>
+    <t>First trans-US rail service begins.</t>
+  </si>
+  <si>
+    <t>First cable car patented, by Andrew Smith Hallidie in the US.</t>
+  </si>
+  <si>
+    <t>First recorded dam disaster in US (Williamsburg, Massachusetts).</t>
+  </si>
+  <si>
+    <t>First cantilever bridge in US completed, Harrodsburg, Kentucky.</t>
+  </si>
+  <si>
+    <t>First female telephone operator starts work (Emma Nutt in Boston).</t>
+  </si>
+  <si>
+    <t>First mobile home (horse drawn) used in a journey from London &amp; Cyprus.</t>
+  </si>
+  <si>
+    <t>World's First electric tram enters service in Lichterfelder (near Berlin).</t>
+  </si>
+  <si>
+    <t>Thomas Stevens is First man to bicycle around the world (San Francisco to San Francisco).</t>
+  </si>
+  <si>
+    <t>San Francisco Bay City Club opens First US bicycle race track, made of wood.</t>
+  </si>
+  <si>
+    <t>America's First auto race organised in Chicago, Frank Duryea wins averaging 7 MPH.</t>
+  </si>
+  <si>
+    <t>First automobile to exceed 100 mph (161 kph), A G MacDonald, Daytona Beach.</t>
+  </si>
+  <si>
+    <t>First railroad accident in US, Granite Railway, Quincy, Massachusetts, kills one.</t>
+  </si>
+  <si>
+    <t>Allardyce Barclay begins a bet of walking one mile every hour for 1,000 hours. Each hour he walked a mile round trip from his home.</t>
+  </si>
+  <si>
+    <t>Streetcar patented (E. A. Gardner of Philadelphia).</t>
+  </si>
+  <si>
+    <t>First mass produced automobile- Henry Ford develops the assembly line method of automobile manufacturing with the introduction of the Ford Model T.</t>
+  </si>
+  <si>
+    <t>First tunnel under Hudson River (railway tunnel) opens.</t>
+  </si>
+  <si>
+    <t>First passenger flight in an airplane.</t>
+  </si>
+  <si>
+    <t>First subway car with side doors goes into service (NYC).</t>
+  </si>
+  <si>
+    <t>First seaplane takes off from water at Martinques France (Henri Fabre).</t>
+  </si>
+  <si>
+    <t>First transcontinental airplane flight, NY-Pasadena in 82 hrs 4 min.</t>
+  </si>
+  <si>
+    <t>Selandia launched – First ocean-going, diesel engine-driven ship.</t>
+  </si>
+  <si>
+    <t>New Mexico becomes 47th state of the Union.</t>
+  </si>
+  <si>
+    <t>Arizona becomes 48th state of the Union.</t>
+  </si>
+  <si>
+    <t>RMS Titanic sets sail from Southampton, England for her maiden (and final) voyage.</t>
+  </si>
+  <si>
+    <t>Grand Central Terminal, the world's largest rail terminal, opens in New York City.</t>
+  </si>
+  <si>
+    <t>Lincoln Highway opens as 1st paved coast-to-coast highway.</t>
+  </si>
+  <si>
+    <t>Panama Canal opens.</t>
+  </si>
+  <si>
+    <t>Motorized scooter invented.</t>
+  </si>
+  <si>
+    <t>The Luftkissengleitboot Hovercraft – First hovering vehicle was created by Dagobert Müller. It could only travel on water.</t>
+  </si>
+  <si>
+    <t>Articulated trams, invented and first used by the Boston Elevated Railway.</t>
+  </si>
+  <si>
+    <t>US Congress passes Federal Aid Road Act.</t>
+  </si>
+  <si>
+    <t>US declares war on Germany, enters World War I.</t>
+  </si>
+  <si>
+    <t>U.S. Civil War begins.</t>
+  </si>
+  <si>
+    <t>U.S. Civil War ends.</t>
+  </si>
+  <si>
+    <t>Wordl War ends.</t>
+  </si>
+  <si>
+    <t>First scheduled passenger service by airplane (Paris-London).</t>
+  </si>
+  <si>
+    <t>First transcontinental airmail flight from New York to San Francisco.</t>
+  </si>
+  <si>
+    <t>First US helium-filled dirigible makes 1st flight.</t>
+  </si>
+  <si>
+    <t>Creation of the USSR formally proclaimed in Moscow.</t>
+  </si>
+  <si>
+    <t>First nonstop north American transcontinental flight (NY-San Diego) completed.</t>
+  </si>
+  <si>
+    <t>First aerial refueling.</t>
+  </si>
+  <si>
+    <t>ZR-1 (biggest active dirigible) flies over NY's tallest skyscraper, Woolworth Tower.</t>
+  </si>
+  <si>
+    <t>First US diesel electric locomotive enters service, Bronx, NY.</t>
+  </si>
+  <si>
+    <t>First road with a depressed trough (Texas) opens to traffic.</t>
+  </si>
+  <si>
+    <t>Robert Goddard launches the first liquid-fueled rocket.</t>
+  </si>
+  <si>
+    <t>U.S. Route 66 is established from Chicago, Illinois to Santa Monica, California 2,448 miles (3,940 km).</t>
+  </si>
+  <si>
+    <t>New York - New Jersey Holland Tunnel, 1st twin-tube underwater auto tunnel, opens.</t>
+  </si>
+  <si>
+    <t>Amelia Earhart becomes the first woman to fly over the Atlantic Ocean.</t>
+  </si>
+  <si>
+    <t>Wall Street Stock Market crashes triggering the "Great Depression.</t>
+  </si>
+  <si>
+    <t>First red &amp; green traffic lights installed in Manhattan, NYC.</t>
+  </si>
+  <si>
+    <t>Congress appropriates $50,000 for Inter-American highway.</t>
+  </si>
+  <si>
+    <t>First air-conditioned train installed-B&amp;O Railroad.</t>
+  </si>
+  <si>
+    <t>First air-conditioned ship (Mariposa) launched.</t>
+  </si>
+  <si>
+    <t>The first electric golf cart was custom-made, but did not gain widespread acceptance.</t>
+  </si>
+  <si>
+    <t>The highest continuous paved road in the United States, the Trail Ridge Road in Rocky Mountain National Park, Colorado, is opened to traffic.</t>
+  </si>
+  <si>
+    <t>Amelia Earhart becomes the first woman to fly solo and nonstop across the Atlantic.</t>
+  </si>
+  <si>
+    <t>First flight of all-metal Boeing 247.</t>
+  </si>
+  <si>
+    <t>Golden Gate Bridge groundbreaking ceremony held at Crissy Field.</t>
+  </si>
+  <si>
+    <t>US Highway planning surveys nationwide authorized.</t>
+  </si>
+  <si>
+    <t>First flight of the DC-3, one of the most significant transport aircraft in the history of aviation.</t>
+  </si>
+  <si>
+    <t>First automatic parking meter in the United States is installed in Oklahoma City, Oklahoma.</t>
+  </si>
+  <si>
+    <t>First bicycle traffic court in America established, Racine, Wisconsin.</t>
+  </si>
+  <si>
+    <t>The Santa Fe Railroad inaugurates the all-Pullman Super Chief passenger train service between Chicago, Illinois and Los Angeles, California.</t>
+  </si>
+  <si>
+    <t>LA Railway Co starts using PCC streetcars.</t>
+  </si>
+  <si>
+    <t>German airship Hindenburg explodes in flames at Lakehurst, New Jersey.</t>
+  </si>
+  <si>
+    <t>The Golden Gate Bridge opens.</t>
+  </si>
+  <si>
+    <t>Appalachian Trail is formally completed, traversing 2,000 miles and 14 US States, Georgia to Maine.</t>
+  </si>
+  <si>
+    <t>Douglas "Wrong Way" Corrigan arrives in Ireland after a 28 hours flight, supposedly left NY flying for California.</t>
+  </si>
+  <si>
+    <t>First jet engine powered aircraft, the Heinkel He 178, takes flight.</t>
+  </si>
+  <si>
+    <t>Lake Washington (Seattle) Floating bridge dedicated.</t>
+  </si>
+  <si>
+    <t>Pennsylvania Turnpike, pioneer toll thruway, opens.</t>
+  </si>
+  <si>
+    <t>First fully articulated bus Isotta Fraschini TS40.</t>
+  </si>
+  <si>
+    <t>The first Jeep is produced.</t>
+  </si>
+  <si>
+    <t>Imperial Japanese Navy with 353 planes attack the US fleet at Pearl Harbor Naval Base, Hawaii, killing 2,403 people.</t>
+  </si>
+  <si>
+    <t>Daylight Savings War Time goes into effect in US.</t>
+  </si>
+  <si>
+    <t>Alaska highway completed.</t>
+  </si>
+  <si>
+    <t>Traffic cone invented.</t>
+  </si>
+  <si>
+    <t>World War II rages.</t>
+  </si>
+  <si>
+    <t>World War II ends.</t>
+  </si>
+  <si>
+    <t>First commercially designed helicopter tested, Bridgeport, Connecticut.</t>
+  </si>
+  <si>
+    <t>First transcontinental round-trip flight in 1-day, California-Maryland.</t>
+  </si>
+  <si>
+    <t>First mobile long-distance car-to-car telephone conversation.</t>
+  </si>
+  <si>
+    <t>Chuck Yeager in the Bell X1 completes the first supersonic manned flight.</t>
+  </si>
+  <si>
+    <t>Maine Turnpike opens to traffic.</t>
+  </si>
+  <si>
+    <t>First radio-controlled airplane flown.</t>
+  </si>
+  <si>
+    <t>Gas turbine-electric locomotive demonstrated at Erie, Pennsylvania.</t>
+  </si>
+  <si>
+    <t>First jet-propelled airline (De Havilland Comet) flies.</t>
+  </si>
+  <si>
+    <t>Brooklyn Battery Tunnel opens in NYC.</t>
+  </si>
+  <si>
+    <t>Golden Gate Bridge closes due to high winds.</t>
+  </si>
+  <si>
+    <t>de Havilland Comet first commercial jet air liner.</t>
+  </si>
+  <si>
+    <t>First west-to-east jet transatlantic nonstop flight</t>
+  </si>
+  <si>
+    <t>Chevrolet unveils V-8 engine.</t>
+  </si>
+  <si>
+    <t>First commercial jet transport plane built in US tested (Boeing 707).</t>
+  </si>
+  <si>
+    <t>First automobile seat belt legislation enacted (Illinois).</t>
+  </si>
+  <si>
+    <t>First nuclear-powered vessel, USS Nautilus, a submarine, is launched.</t>
+  </si>
+  <si>
+    <t>Interstate highway system begins with the signing of the Federal-Aid Highway Act.</t>
+  </si>
+  <si>
+    <t>Sputnik 1 – First artificial satellite to be launched into orbit.</t>
+  </si>
+  <si>
+    <t>Ford Motor Co. introduces Edsel.</t>
+  </si>
+  <si>
+    <t>First appearance of "In God We Trust" on U.S. paper currency.</t>
+  </si>
+  <si>
+    <t>First airplane flight exceeding 1200 hours, lands, Dallas TX.</t>
+  </si>
+  <si>
+    <t>Alaska becomes 49th state of the Union.</t>
+  </si>
+  <si>
+    <t>Hawaii becomes 50th state of the Union.</t>
+  </si>
+  <si>
+    <t>The St. Lawrence Seaway is opened along the Canada and United States.</t>
+  </si>
+  <si>
+    <t>Europe's first "moving pavement" (travelator), opens at Bank station on the London Underground.</t>
+  </si>
+  <si>
+    <t>The first U.S. manned sub-orbital space flight is completed with Commander Alan B. Shepard Jr.</t>
+  </si>
+  <si>
+    <t>The Cuban Missile Crises.</t>
+  </si>
+  <si>
+    <t>John Glenn becomes the 1st American to orbit the Earth, aboard Friendship 7.</t>
+  </si>
+  <si>
+    <t>Massachusetts Institute of Technology sends TV signal by satellite for 1st time: California to Massachusetts.</t>
+  </si>
+  <si>
+    <t>LA ends streetcar service after 90 years.</t>
+  </si>
+  <si>
+    <t>France &amp; Great-Britain sign accord over building channel tunnel.</t>
+  </si>
+  <si>
+    <t>First driverless trains run on London Underground.</t>
+  </si>
+  <si>
+    <t>First ground station-to-aircraft radio communication via satellite.</t>
+  </si>
+  <si>
+    <t>Gemini 8 launched with Armstrong &amp; Scott, aborted after 6.5 orbits.</t>
+  </si>
+  <si>
+    <t>Sheila Scott completes 1st round-the-world solo flight by a woman.</t>
+  </si>
+  <si>
+    <t>Carl Sagan turns 1 billion seconds old.</t>
+  </si>
+  <si>
+    <t>A fire in the Apollo 1 Command Module kills astronauts Gus Grissom, Ed White and Roger B. Chaffee during a launch rehearsal.</t>
+  </si>
+  <si>
+    <t>First air conditioned NYC subway car (R-38 on the F line).</t>
+  </si>
+  <si>
+    <t>Sweden switches to driving on the right hand side.</t>
+  </si>
+  <si>
+    <t>The formal end of steam traction in the North East of England by British Railways.</t>
+  </si>
+  <si>
+    <t>Ferdinand Bracke bicycles world record time (48,093 km).</t>
+  </si>
+  <si>
+    <t>Supersonic airliner prototype "Concorde" 1st shown (France).</t>
+  </si>
+  <si>
+    <t>Space hopper (childs toy) invented.</t>
+  </si>
+  <si>
+    <t>First Boeing 747 rolls out.</t>
+  </si>
+  <si>
+    <t>Golden Gate Bridge charges tolls only for southbound cars.</t>
+  </si>
+  <si>
+    <t>Apollo 8: First manned Moon voyage launched with Frank Borman, Jim Lovell and William Anders.</t>
+  </si>
+  <si>
+    <t>First flight of the Boeing 747.</t>
+  </si>
+  <si>
+    <t>Apollo 11 launched, carrying 1st men to land on Moon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Apollo 13 launched to Moon; unable to land, returns in 6 days.</t>
+  </si>
+  <si>
+    <t>Salyut 1, first space station, launched by Soviet Union.</t>
+  </si>
+  <si>
+    <t>Amtrak Railroad begins operation.</t>
+  </si>
+  <si>
+    <t>First flight of the Goodyear blimp.</t>
+  </si>
+  <si>
+    <t>The Bosphorus Bridge in Istanbul, Turkey is completed, connecting the continents of Europe and Asia over the Bosporus for the first time.</t>
+  </si>
+  <si>
+    <t>In response to the 1973 energy crisis, daylight saving time commences nearly four months early in the United States.</t>
+  </si>
+  <si>
+    <t>BART begins regular transbay service.</t>
+  </si>
+  <si>
+    <t>West Virginia-Morgantown PRT, first Personal Rapid Transit system to be installed.</t>
+  </si>
+  <si>
+    <t>Apollo 18 and Soyuz 19 make 1st US/USSR linkup in space.</t>
+  </si>
+  <si>
+    <t>The Viking 1 &amp; 2 space probes successfully land on Mars.</t>
+  </si>
+  <si>
+    <t>Longest non-stop passenger airflight (Sydney to San Francisco 13h 14m).</t>
+  </si>
+  <si>
+    <t>The first semi-automated car was developed in 1977, by Japan's Tsukuba Mechanical Engineering Laboratory.</t>
+  </si>
+  <si>
+    <t>Space Shuttle Enterprise takes its maiden flight affixed atop a Boeing 747 Shuttle Aircraft Carrier.</t>
+  </si>
+  <si>
+    <t>Final European scheduled run of the Orient Express (after 94 years).</t>
+  </si>
+  <si>
+    <t>Orient Express opens.</t>
+  </si>
+  <si>
+    <t>US Railway Post Office final train run (NY to Washington, D.C.).</t>
+  </si>
+  <si>
+    <t>Voyager 1 (US) launched toward fly-by of Jupiter, Saturn.</t>
+  </si>
+  <si>
+    <t>Pioneer 11 transmits images of Saturn and its rings.</t>
+  </si>
+  <si>
+    <t>US Skylab enters atmosphere over Australia and disintegrates.</t>
+  </si>
+  <si>
+    <t>Skylab was the first United States space station, launched by NASA.</t>
+  </si>
+  <si>
+    <t>Voyager 1 space probe discovers 15th moon of Saturn.</t>
+  </si>
+  <si>
+    <t>Maiden flight of the Space Shuttle.</t>
+  </si>
+  <si>
+    <t>The first fully Automated guideway transit driverless people mover train technology introduced on Port Island Line, Japan.</t>
+  </si>
+  <si>
+    <t>Concorde makes the world's first commercial passenger-carrying supersonic flight.</t>
+  </si>
+  <si>
+    <t>First non-stop trans-North American balloon flight departs Fort Baker, California. Maxie Anderson and son Kristian pilot the Kitty Hawk for five days.</t>
+  </si>
+  <si>
+    <t>Waterfront streetcar begins operating in Seattle.</t>
+  </si>
+  <si>
+    <t>Manhattan, NY institutes bus-only lanes.</t>
+  </si>
+  <si>
+    <t>Streetcars stop running on Market St, San Francisco after 122 years of service.</t>
+  </si>
+  <si>
+    <t>San Francisco cable cars cease operations for 2 years of repairs.</t>
+  </si>
+  <si>
+    <t>First Automated guideway transit driverless metro, Véhicule Automatique Léger introduced in Lille Metro, France.</t>
+  </si>
+  <si>
+    <t>First commercial maglev, albeit low-speed opens in Birmingham.</t>
+  </si>
+  <si>
+    <t>US government orders air bags or seat belts would be required in cars by 1989.</t>
+  </si>
+  <si>
+    <t>Sinclair C5, the first mass-produced electric battery velomobile launched.</t>
+  </si>
+  <si>
+    <t>The Challenger Space Shuttle explodes after lift off at Cape Canaveral, Florida, killing seven people, including Christa McAuliffe, a New Hampshire school teacher.</t>
+  </si>
+  <si>
+    <t>Chunnel announced (railroad tunnel under English Channel).</t>
+  </si>
+  <si>
+    <t>Voyager, piloted by Dick Rutan &amp; Jeana Yeager, takes off from Edwards AFB, California on 1st non-stop, non-refueled flight around the world.</t>
+  </si>
+  <si>
+    <t>Two men became 1st hot-air balloon travelers to cross Atlantic.</t>
+  </si>
+  <si>
+    <t>United Airlines Boeing 747SP, circles world in 36h 54m 15s.</t>
+  </si>
+  <si>
+    <t>Boston's worst traffic jam in 30 years. (Jul 27)</t>
+  </si>
+  <si>
+    <t>Union Station reopens in Washington, D.C.</t>
+  </si>
+  <si>
+    <t>NYC Subway system adds new stations (Z line).</t>
+  </si>
+  <si>
+    <t>Last graffiti covered NYC subway car retired.</t>
+  </si>
+  <si>
+    <t>Longest Cab Ride Ever: 14,000 miles costs $16,000!</t>
+  </si>
+  <si>
+    <t>NASA  Voyager 2's discovered three more moons of Neptune and  two rings.</t>
+  </si>
+  <si>
+    <t>ADtranz low floor tram world's first completely low-floor tram introduced.</t>
+  </si>
+  <si>
+    <t>The Intermodal Surface Transportation Efficiency Act posed a major change to transportation planning and policy, as the first U.S. federal legislation in the post-Interstate Highway System era.</t>
+  </si>
+  <si>
+    <t>Key bus route progam of the (MBTA) rolled out. The Key bus routes are 15 routes that have high ridership and higher frequency.</t>
+  </si>
+  <si>
+    <t>The CharlieCard debutes. It is a contactless smart card on which the passenger loads fares. It replaces the metal token.</t>
+  </si>
+  <si>
+    <t>Covid pandemic.</t>
+  </si>
+  <si>
+    <t>Channel Tunnel opens.</t>
+  </si>
+  <si>
+    <t>First Maglev train prototypes are tested in Japan.</t>
+  </si>
+  <si>
+    <t>Honda Raccoon Compo, first folding electric bicycle in Japan.</t>
+  </si>
+  <si>
+    <t>Trikke (wiggle scooter) invented.</t>
+  </si>
+  <si>
+    <t>US space probe Ulyssus completes 2nd passage behind Sun.</t>
+  </si>
+  <si>
+    <t>Segway PT self-balancing personal transport was launched by inventor Dean Kamen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> First commercial high speed Maglev train starts operation between Shanghai and its airport.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tesla Roadster, first mass production lithium-ion battery electric car.</t>
+  </si>
+  <si>
+    <t>First mass produced hydrogen fuel cell car, Toyota Mirai.</t>
+  </si>
+  <si>
+    <t>Conventional rail world speed record of 443.0 km/h (275.3 mph) attained by the JR Central "300X" six-car train between Kyoto and Maibara on the Tokaido Shinkansen.</t>
+  </si>
+  <si>
+    <t>Amtrak extends electric train operation on the Northeast Corridor from New Haven to Boston South Station.</t>
+  </si>
+  <si>
+    <t>Concorde makes last passenger flight.</t>
+  </si>
+  <si>
+    <t>The Downeaster, a passenger train operated by Amtrak, begins regularly scheduled passenger service between Boston, Massachusetts and Portland, Maine.</t>
+  </si>
+  <si>
+    <t>The Girard Avenue Trolley in Philadelphia recommences service after thirteen years of bus substitution.</t>
+  </si>
+  <si>
+    <t>Construction begins on the Second Avenue Subway in New York City between 63rd and 105th streets, a resumption of a decades-long project with existing segments elsewhere.</t>
+  </si>
+  <si>
+    <t>Sound Transit Central Link light rail line in Seattle, Washington opens, utilizing the Downtown Seattle Transit Tunnel.</t>
+  </si>
+  <si>
+    <t>ULTra (rapid transit), the first modern commercial Personal Rapid Transit system to be installed. Started operations at Heathrow Airport.</t>
+  </si>
+  <si>
+    <t>Brookhaven Rail Terminal opened on Long Island, New York.</t>
+  </si>
+  <si>
+    <t>The first phase of Los Angeles County Metropolitan Transportation Authority Expo Line opens for service.</t>
+  </si>
+  <si>
+    <t>New Orleans Regional Transit Authority Loyola Avenue Streetcar Line opened.</t>
+  </si>
+  <si>
+    <t>Opening of the Green Line light rail service in Minneapolis–Saint Paul, Minnesota.</t>
+  </si>
+  <si>
+    <t>Opening of the MAX Orange Line in Portland, Oregon, United States.</t>
+  </si>
+  <si>
+    <t>Opening of the B Line commuter rail system in Denver, Colorado.</t>
+  </si>
+  <si>
+    <t>Opening of Detroit's QLINE.</t>
+  </si>
+  <si>
+    <t>Autonomous Rail Rapid Transit opened in China.</t>
+  </si>
+  <si>
+    <t>The Washington Metro Silver Line extended to Ashburn station via Washington Dulles International Airport.</t>
+  </si>
+  <si>
+    <t>The first segment of the Southern California Rapid Transit District Red Line subway opens in Los Angeles.</t>
+  </si>
+  <si>
+    <t>Southern California's Metrolink opens.</t>
   </si>
   <si>
     <t>year</t>
@@ -885,9 +1506,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8479D0E-E3F6-DA41-AEC9-2CE4981D9A6E}">
-  <dimension ref="A1:B160"/>
+  <dimension ref="A1:B367"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -897,10 +1520,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>157</v>
+        <v>364</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>158</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -916,7 +1539,7 @@
         <v>1800</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>156</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -924,7 +1547,7 @@
         <v>1801</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -932,7 +1555,7 @@
         <v>1801</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>154</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -940,7 +1563,7 @@
         <v>1802</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -948,7 +1571,7 @@
         <v>1803</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -956,7 +1579,7 @@
         <v>1803</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>151</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1012,7 +1635,7 @@
         <v>1807</v>
       </c>
       <c r="B15" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1036,7 +1659,7 @@
         <v>1807</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1044,7 +1667,7 @@
         <v>1808</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1052,7 +1675,7 @@
         <v>1809</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1068,7 +1691,7 @@
         <v>1809</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1076,7 +1699,7 @@
         <v>1810</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1084,7 +1707,7 @@
         <v>1811</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1092,7 +1715,7 @@
         <v>1812</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1100,7 +1723,7 @@
         <v>1812</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1108,7 +1731,7 @@
         <v>1812</v>
       </c>
       <c r="B27" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1116,7 +1739,7 @@
         <v>1813</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1124,7 +1747,7 @@
         <v>1814</v>
       </c>
       <c r="B29" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1132,7 +1755,7 @@
         <v>1814</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1140,7 +1763,7 @@
         <v>1815</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1148,7 +1771,7 @@
         <v>1816</v>
       </c>
       <c r="B32" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1164,7 +1787,7 @@
         <v>1817</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1172,7 +1795,7 @@
         <v>1817</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1180,7 +1803,7 @@
         <v>1818</v>
       </c>
       <c r="B36" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1188,7 +1811,7 @@
         <v>1818</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1196,7 +1819,7 @@
         <v>1819</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1204,7 +1827,7 @@
         <v>1819</v>
       </c>
       <c r="B39" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1212,7 +1835,7 @@
         <v>1819</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1220,7 +1843,7 @@
         <v>1819</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1228,7 +1851,7 @@
         <v>1819</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1236,7 +1859,7 @@
         <v>1820</v>
       </c>
       <c r="B43" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1244,7 +1867,7 @@
         <v>1820</v>
       </c>
       <c r="B44" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1252,7 +1875,7 @@
         <v>1821</v>
       </c>
       <c r="B45" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1260,7 +1883,7 @@
         <v>1822</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1268,7 +1891,7 @@
         <v>1823</v>
       </c>
       <c r="B47" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1276,7 +1899,7 @@
         <v>1823</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1284,7 +1907,7 @@
         <v>1824</v>
       </c>
       <c r="B49" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1292,7 +1915,7 @@
         <v>1825</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1300,7 +1923,7 @@
         <v>1825</v>
       </c>
       <c r="B51" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1308,7 +1931,7 @@
         <v>1826</v>
       </c>
       <c r="B52" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1316,7 +1939,7 @@
         <v>1827</v>
       </c>
       <c r="B53" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1324,7 +1947,7 @@
         <v>1827</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1332,7 +1955,7 @@
         <v>1828</v>
       </c>
       <c r="B55" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1340,7 +1963,7 @@
         <v>1828</v>
       </c>
       <c r="B56" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1348,7 +1971,7 @@
         <v>1829</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1356,7 +1979,7 @@
         <v>1829</v>
       </c>
       <c r="B58" t="s">
-        <v>37</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1364,7 +1987,7 @@
         <v>1830</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1372,7 +1995,7 @@
         <v>1830</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1380,7 +2003,7 @@
         <v>1830</v>
       </c>
       <c r="B61" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1388,7 +2011,7 @@
         <v>1830</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1396,7 +2019,7 @@
         <v>1831</v>
       </c>
       <c r="B63" t="s">
-        <v>42</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1404,7 +2027,7 @@
         <v>1831</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1412,7 +2035,7 @@
         <v>1831</v>
       </c>
       <c r="B65" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1420,7 +2043,7 @@
         <v>1832</v>
       </c>
       <c r="B66" t="s">
-        <v>45</v>
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1428,7 +2051,7 @@
         <v>1832</v>
       </c>
       <c r="B67" t="s">
-        <v>46</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1436,7 +2059,7 @@
         <v>1833</v>
       </c>
       <c r="B68" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1444,7 +2067,7 @@
         <v>1834</v>
       </c>
       <c r="B69" t="s">
-        <v>48</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1452,7 +2075,7 @@
         <v>1835</v>
       </c>
       <c r="B70" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1460,7 +2083,7 @@
         <v>1836</v>
       </c>
       <c r="B71" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1468,7 +2091,7 @@
         <v>1837</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1476,7 +2099,7 @@
         <v>1837</v>
       </c>
       <c r="B73" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1484,7 +2107,7 @@
         <v>1837</v>
       </c>
       <c r="B74" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1492,7 +2115,7 @@
         <v>1837</v>
       </c>
       <c r="B75" t="s">
-        <v>54</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1500,7 +2123,7 @@
         <v>1838</v>
       </c>
       <c r="B76" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1508,7 +2131,7 @@
         <v>1839</v>
       </c>
       <c r="B77" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1516,7 +2139,7 @@
         <v>1839</v>
       </c>
       <c r="B78" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1524,7 +2147,7 @@
         <v>1840</v>
       </c>
       <c r="B79" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1532,7 +2155,7 @@
         <v>1841</v>
       </c>
       <c r="B80" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1540,7 +2163,7 @@
         <v>1842</v>
       </c>
       <c r="B81" t="s">
-        <v>62</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1548,7 +2171,7 @@
         <v>1843</v>
       </c>
       <c r="B82" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1556,7 +2179,7 @@
         <v>1844</v>
       </c>
       <c r="B83" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1564,7 +2187,7 @@
         <v>1845</v>
       </c>
       <c r="B84" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1572,7 +2195,7 @@
         <v>1845</v>
       </c>
       <c r="B85" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1580,7 +2203,7 @@
         <v>1845</v>
       </c>
       <c r="B86" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1588,7 +2211,7 @@
         <v>1846</v>
       </c>
       <c r="B87" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1596,7 +2219,7 @@
         <v>1847</v>
       </c>
       <c r="B88" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1604,7 +2227,7 @@
         <v>1848</v>
       </c>
       <c r="B89" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1612,7 +2235,7 @@
         <v>1848</v>
       </c>
       <c r="B90" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1620,7 +2243,7 @@
         <v>1849</v>
       </c>
       <c r="B91" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1628,7 +2251,7 @@
         <v>1850</v>
       </c>
       <c r="B92" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1636,7 +2259,7 @@
         <v>1851</v>
       </c>
       <c r="B93" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1644,7 +2267,7 @@
         <v>1852</v>
       </c>
       <c r="B94" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1652,7 +2275,7 @@
         <v>1852</v>
       </c>
       <c r="B95" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1660,7 +2283,7 @@
         <v>1853</v>
       </c>
       <c r="B96" t="s">
-        <v>77</v>
+        <v>149</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1668,7 +2291,7 @@
         <v>1853</v>
       </c>
       <c r="B97" t="s">
-        <v>78</v>
+        <v>150</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1676,7 +2299,7 @@
         <v>1854</v>
       </c>
       <c r="B98" t="s">
-        <v>82</v>
+        <v>151</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1684,7 +2307,7 @@
         <v>1855</v>
       </c>
       <c r="B99" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1692,7 +2315,7 @@
         <v>1855</v>
       </c>
       <c r="B100" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1700,7 +2323,7 @@
         <v>1855</v>
       </c>
       <c r="B101" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -1708,7 +2331,7 @@
         <v>1856</v>
       </c>
       <c r="B102" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -1716,7 +2339,7 @@
         <v>1857</v>
       </c>
       <c r="B103" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -1724,7 +2347,7 @@
         <v>1858</v>
       </c>
       <c r="B104" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -1732,7 +2355,7 @@
         <v>1858</v>
       </c>
       <c r="B105" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -1740,7 +2363,7 @@
         <v>1858</v>
       </c>
       <c r="B106" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -1748,7 +2371,7 @@
         <v>1859</v>
       </c>
       <c r="B107" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -1756,7 +2379,7 @@
         <v>1859</v>
       </c>
       <c r="B108" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -1764,7 +2387,7 @@
         <v>1859</v>
       </c>
       <c r="B109" t="s">
-        <v>89</v>
+        <v>155</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -1772,7 +2395,7 @@
         <v>1860</v>
       </c>
       <c r="B110" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -1780,7 +2403,7 @@
         <v>1861</v>
       </c>
       <c r="B111" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -1788,23 +2411,23 @@
         <v>1861</v>
       </c>
       <c r="B112" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="B113" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="B114" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -1812,39 +2435,39 @@
         <v>1863</v>
       </c>
       <c r="B115" t="s">
-        <v>95</v>
+        <v>156</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="B116" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="B117" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="B118" t="s">
-        <v>98</v>
+        <v>193</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="B119" t="s">
-        <v>99</v>
+        <v>157</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -1852,15 +2475,15 @@
         <v>1867</v>
       </c>
       <c r="B120" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="B121" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -1868,15 +2491,15 @@
         <v>1868</v>
       </c>
       <c r="B122" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="B123" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -1884,31 +2507,31 @@
         <v>1869</v>
       </c>
       <c r="B124" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="B125" t="s">
-        <v>104</v>
+        <v>159</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="B126" t="s">
-        <v>105</v>
+        <v>160</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="B127" t="s">
-        <v>106</v>
+        <v>161</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -1916,47 +2539,47 @@
         <v>1872</v>
       </c>
       <c r="B128" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="B129" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="B130" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="B131" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="B132" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="B133" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -1964,111 +2587,111 @@
         <v>1877</v>
       </c>
       <c r="B134" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="B135" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="B136" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="B137" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="B138" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="B139" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="B140" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="B141" t="s">
-        <v>138</v>
+        <v>301</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>1885</v>
+        <v>1883</v>
       </c>
       <c r="B142" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>1886</v>
+        <v>1884</v>
       </c>
       <c r="B143" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>1887</v>
+        <v>1885</v>
       </c>
       <c r="B144" t="s">
-        <v>122</v>
+        <v>80</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>1888</v>
+        <v>1886</v>
       </c>
       <c r="B145" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>1889</v>
+        <v>1887</v>
       </c>
       <c r="B146" t="s">
-        <v>124</v>
+        <v>167</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B147" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -2076,7 +2699,7 @@
         <v>1889</v>
       </c>
       <c r="B148" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -2084,55 +2707,55 @@
         <v>1889</v>
       </c>
       <c r="B149" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="B150" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="B151" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="B152" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>1892</v>
+        <v>1890</v>
       </c>
       <c r="B153" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>1893</v>
+        <v>1891</v>
       </c>
       <c r="B154" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="B155" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -2140,39 +2763,1695 @@
         <v>1893</v>
       </c>
       <c r="B156" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="B157" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>1895</v>
+        <v>1893</v>
       </c>
       <c r="B158" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="B159" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
+        <v>1895</v>
+      </c>
+      <c r="B160" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>1895</v>
+      </c>
+      <c r="B161" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
         <v>1896</v>
       </c>
-      <c r="B160" t="s">
-        <v>135</v>
+      <c r="B162" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>1897</v>
+      </c>
+      <c r="B163" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>1897</v>
+      </c>
+      <c r="B164" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>1898</v>
+      </c>
+      <c r="B165" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>1898</v>
+      </c>
+      <c r="B166" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>1899</v>
+      </c>
+      <c r="B167" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>1900</v>
+      </c>
+      <c r="B168" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>1900</v>
+      </c>
+      <c r="B169" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>1901</v>
+      </c>
+      <c r="B170" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>1902</v>
+      </c>
+      <c r="B171" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>1903</v>
+      </c>
+      <c r="B172" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>1903</v>
+      </c>
+      <c r="B173" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>1904</v>
+      </c>
+      <c r="B174" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>1904</v>
+      </c>
+      <c r="B175" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>1904</v>
+      </c>
+      <c r="B176" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>1905</v>
+      </c>
+      <c r="B177" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>1906</v>
+      </c>
+      <c r="B178" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <v>1907</v>
+      </c>
+      <c r="B179" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>1907</v>
+      </c>
+      <c r="B180" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>1908</v>
+      </c>
+      <c r="B181" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>1908</v>
+      </c>
+      <c r="B182" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>1908</v>
+      </c>
+      <c r="B183" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>1909</v>
+      </c>
+      <c r="B184" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>1910</v>
+      </c>
+      <c r="B185" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>1911</v>
+      </c>
+      <c r="B186" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>1911</v>
+      </c>
+      <c r="B187" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>1912</v>
+      </c>
+      <c r="B188" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>1912</v>
+      </c>
+      <c r="B189" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>1912</v>
+      </c>
+      <c r="B190" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>1912</v>
+      </c>
+      <c r="B191" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>1913</v>
+      </c>
+      <c r="B192" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>1913</v>
+      </c>
+      <c r="B193" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>1914</v>
+      </c>
+      <c r="B194" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>1915</v>
+      </c>
+      <c r="B195" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>1915</v>
+      </c>
+      <c r="B196" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>1916</v>
+      </c>
+      <c r="B197" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>1917</v>
+      </c>
+      <c r="B198" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>1918</v>
+      </c>
+      <c r="B199" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>1919</v>
+      </c>
+      <c r="B200" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>1920</v>
+      </c>
+      <c r="B201" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>1921</v>
+      </c>
+      <c r="B202" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>1922</v>
+      </c>
+      <c r="B203" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>1923</v>
+      </c>
+      <c r="B204" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>1923</v>
+      </c>
+      <c r="B205" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>1923</v>
+      </c>
+      <c r="B206" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>1924</v>
+      </c>
+      <c r="B207" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>1925</v>
+      </c>
+      <c r="B208" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>1926</v>
+      </c>
+      <c r="B209" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>1926</v>
+      </c>
+      <c r="B210" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="1">
+        <v>1927</v>
+      </c>
+      <c r="B211" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>1928</v>
+      </c>
+      <c r="B212" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>1929</v>
+      </c>
+      <c r="B213" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>1930</v>
+      </c>
+      <c r="B214" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>1930</v>
+      </c>
+      <c r="B215" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" s="1">
+        <v>1931</v>
+      </c>
+      <c r="B216" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>1931</v>
+      </c>
+      <c r="B217" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
+        <v>1932</v>
+      </c>
+      <c r="B218" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>1932</v>
+      </c>
+      <c r="B219" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>1932</v>
+      </c>
+      <c r="B220" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>1933</v>
+      </c>
+      <c r="B221" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>1933</v>
+      </c>
+      <c r="B222" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>1934</v>
+      </c>
+      <c r="B223" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="1">
+        <v>1935</v>
+      </c>
+      <c r="B224" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" s="1">
+        <v>1935</v>
+      </c>
+      <c r="B225" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" s="1">
+        <v>1936</v>
+      </c>
+      <c r="B226" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" s="1">
+        <v>1936</v>
+      </c>
+      <c r="B227" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>1937</v>
+      </c>
+      <c r="B228" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>1937</v>
+      </c>
+      <c r="B229" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
+        <v>1937</v>
+      </c>
+      <c r="B230" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
+        <v>1937</v>
+      </c>
+      <c r="B231" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" s="1">
+        <v>1938</v>
+      </c>
+      <c r="B232" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>1939</v>
+      </c>
+      <c r="B233" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" s="1">
+        <v>1940</v>
+      </c>
+      <c r="B234" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="1">
+        <v>1940</v>
+      </c>
+      <c r="B235" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" s="1">
+        <v>1940</v>
+      </c>
+      <c r="B236" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" s="1">
+        <v>1941</v>
+      </c>
+      <c r="B237" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" s="1">
+        <v>1941</v>
+      </c>
+      <c r="B238" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" s="1">
+        <v>1942</v>
+      </c>
+      <c r="B239" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>1942</v>
+      </c>
+      <c r="B240" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>1943</v>
+      </c>
+      <c r="B241" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
+        <v>1944</v>
+      </c>
+      <c r="B242" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
+        <v>1945</v>
+      </c>
+      <c r="B243" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" s="1">
+        <v>1946</v>
+      </c>
+      <c r="B244" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
+        <v>1946</v>
+      </c>
+      <c r="B245" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>1946</v>
+      </c>
+      <c r="B246" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
+        <v>1947</v>
+      </c>
+      <c r="B247" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>1947</v>
+      </c>
+      <c r="B248" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
+        <v>1948</v>
+      </c>
+      <c r="B249" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="1">
+        <v>1949</v>
+      </c>
+      <c r="B250" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="1">
+        <v>1949</v>
+      </c>
+      <c r="B251" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
+        <v>1950</v>
+      </c>
+      <c r="B252" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="1">
+        <v>1951</v>
+      </c>
+      <c r="B253" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" s="1">
+        <v>1952</v>
+      </c>
+      <c r="B254" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
+        <v>1953</v>
+      </c>
+      <c r="B255" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" s="1">
+        <v>1954</v>
+      </c>
+      <c r="B256" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" s="1">
+        <v>1954</v>
+      </c>
+      <c r="B257" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" s="1">
+        <v>1955</v>
+      </c>
+      <c r="B258" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" s="1">
+        <v>1955</v>
+      </c>
+      <c r="B259" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" s="1">
+        <v>1956</v>
+      </c>
+      <c r="B260" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" s="1">
+        <v>1957</v>
+      </c>
+      <c r="B261" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" s="1">
+        <v>1957</v>
+      </c>
+      <c r="B262" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" s="1">
+        <v>1957</v>
+      </c>
+      <c r="B263" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" s="1">
+        <v>1958</v>
+      </c>
+      <c r="B264" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" s="1">
+        <v>1959</v>
+      </c>
+      <c r="B265" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" s="1">
+        <v>1959</v>
+      </c>
+      <c r="B266" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" s="1">
+        <v>1959</v>
+      </c>
+      <c r="B267" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" s="1">
+        <v>1960</v>
+      </c>
+      <c r="B268" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" s="1">
+        <v>1961</v>
+      </c>
+      <c r="B269" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" s="1">
+        <v>1962</v>
+      </c>
+      <c r="B270" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" s="1">
+        <v>1962</v>
+      </c>
+      <c r="B271" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" s="1">
+        <v>1962</v>
+      </c>
+      <c r="B272" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" s="1">
+        <v>1963</v>
+      </c>
+      <c r="B273" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" s="1">
+        <v>1964</v>
+      </c>
+      <c r="B274" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" s="1">
+        <v>1964</v>
+      </c>
+      <c r="B275" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" s="1">
+        <v>1965</v>
+      </c>
+      <c r="B276" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" s="1">
+        <v>1966</v>
+      </c>
+      <c r="B277" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" s="1">
+        <v>1966</v>
+      </c>
+      <c r="B278" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="1">
+        <v>1966</v>
+      </c>
+      <c r="B279" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="1">
+        <v>1967</v>
+      </c>
+      <c r="B280" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="1">
+        <v>1967</v>
+      </c>
+      <c r="B281" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="1">
+        <v>1967</v>
+      </c>
+      <c r="B282" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" s="1">
+        <v>1967</v>
+      </c>
+      <c r="B283" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" s="1">
+        <v>1967</v>
+      </c>
+      <c r="B284" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" s="1">
+        <v>1967</v>
+      </c>
+      <c r="B285" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" s="1">
+        <v>1968</v>
+      </c>
+      <c r="B286" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" s="1">
+        <v>1968</v>
+      </c>
+      <c r="B287" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" s="1">
+        <v>1968</v>
+      </c>
+      <c r="B288" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" s="1">
+        <v>1968</v>
+      </c>
+      <c r="B289" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" s="1">
+        <v>1969</v>
+      </c>
+      <c r="B290" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" s="1">
+        <v>1969</v>
+      </c>
+      <c r="B291" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" s="1">
+        <v>1970</v>
+      </c>
+      <c r="B292" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" s="1">
+        <v>1971</v>
+      </c>
+      <c r="B293" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" s="1">
+        <v>1971</v>
+      </c>
+      <c r="B294" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" s="1">
+        <v>1972</v>
+      </c>
+      <c r="B295" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" s="1">
+        <v>1973</v>
+      </c>
+      <c r="B296" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" s="1">
+        <v>1973</v>
+      </c>
+      <c r="B297" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" s="1">
+        <v>1974</v>
+      </c>
+      <c r="B298" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" s="1">
+        <v>1974</v>
+      </c>
+      <c r="B299" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" s="1">
+        <v>1975</v>
+      </c>
+      <c r="B300" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" s="1">
+        <v>1975</v>
+      </c>
+      <c r="B301" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" s="1">
+        <v>1976</v>
+      </c>
+      <c r="B302" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" s="1">
+        <v>1976</v>
+      </c>
+      <c r="B303" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" s="1">
+        <v>1976</v>
+      </c>
+      <c r="B304" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" s="1">
+        <v>1977</v>
+      </c>
+      <c r="B305" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" s="1">
+        <v>1977</v>
+      </c>
+      <c r="B306" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" s="1">
+        <v>1977</v>
+      </c>
+      <c r="B307" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308" s="1">
+        <v>1977</v>
+      </c>
+      <c r="B308" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309" s="1">
+        <v>1977</v>
+      </c>
+      <c r="B309" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310" s="1">
+        <v>1978</v>
+      </c>
+      <c r="B310" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311" s="1">
+        <v>1979</v>
+      </c>
+      <c r="B311" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" s="1">
+        <v>1980</v>
+      </c>
+      <c r="B312" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313" s="1">
+        <v>1980</v>
+      </c>
+      <c r="B313" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" s="1">
+        <v>1981</v>
+      </c>
+      <c r="B314" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" s="1">
+        <v>1981</v>
+      </c>
+      <c r="B315" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" s="1">
+        <v>1982</v>
+      </c>
+      <c r="B316" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" s="1">
+        <v>1982</v>
+      </c>
+      <c r="B317" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318" s="1">
+        <v>1982</v>
+      </c>
+      <c r="B318" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319" s="1">
+        <v>1982</v>
+      </c>
+      <c r="B319" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" s="1">
+        <v>1983</v>
+      </c>
+      <c r="B320" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" s="1">
+        <v>1984</v>
+      </c>
+      <c r="B321" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" s="1">
+        <v>1984</v>
+      </c>
+      <c r="B322" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" s="1">
+        <v>1985</v>
+      </c>
+      <c r="B323" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" s="1">
+        <v>1986</v>
+      </c>
+      <c r="B324" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" s="1">
+        <v>1986</v>
+      </c>
+      <c r="B325" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" s="1">
+        <v>1986</v>
+      </c>
+      <c r="B326" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" s="1">
+        <v>1987</v>
+      </c>
+      <c r="B327" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" s="1">
+        <v>1988</v>
+      </c>
+      <c r="B328" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" s="1">
+        <v>1988</v>
+      </c>
+      <c r="B329" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" s="1">
+        <v>1988</v>
+      </c>
+      <c r="B330" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" s="1">
+        <v>1988</v>
+      </c>
+      <c r="B331" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" s="1">
+        <v>1989</v>
+      </c>
+      <c r="B332" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" s="1">
+        <v>1989</v>
+      </c>
+      <c r="B333" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" s="1">
+        <v>1989</v>
+      </c>
+      <c r="B334" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B335" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B336" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B337" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B338" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B339" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B340" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B341" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B342" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B343" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B344" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B345" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B346" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B347" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B348" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B349" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B350" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B351" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B352" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B353" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B354" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B355" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B356" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B357" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B358" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B359" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B360" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B361" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B362" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B363" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B364" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B365" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B366" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B367" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
One additional historical fact from Jonathan Belcher added.
</commit_message>
<xml_diff>
--- a/xlsx/historical_items.xlsx
+++ b/xlsx/historical_items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C41B2E-235A-4E81-BCD7-EEB0E420EDFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FAFB99-37DB-4238-BD25-9D362BDE89BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{171EF181-1F3C-7A42-9B63-D835B687641B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="656">
   <si>
     <t>The U.S. capital is moved from Philadelphia to Washington, DC.</t>
   </si>
@@ -1990,6 +1990,9 @@
   </si>
   <si>
     <t>MBTA Green Line A branch converted to 57 bus in June.</t>
+  </si>
+  <si>
+    <t>The relocated northern portion of the MBTA Orange line opened to Sullivan in April, to Wellington in September, and to Malden in December.</t>
   </si>
 </sst>
 </file>
@@ -2376,10 +2379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8479D0E-E3F6-DA41-AEC9-2CE4981D9A6E}">
-  <dimension ref="A1:B655"/>
+  <dimension ref="A1:B656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A487" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A503" sqref="A503"/>
+    <sheetView tabSelected="1" topLeftCell="A511" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B520" sqref="B520"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6537,7 +6540,7 @@
         <v>1975</v>
       </c>
       <c r="B519" t="s">
-        <v>485</v>
+        <v>655</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
@@ -6545,7 +6548,7 @@
         <v>1975</v>
       </c>
       <c r="B520" t="s">
-        <v>268</v>
+        <v>485</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.25">
@@ -6553,15 +6556,15 @@
         <v>1975</v>
       </c>
       <c r="B521" t="s">
-        <v>596</v>
+        <v>268</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A522" s="1">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="B522" t="s">
-        <v>486</v>
+        <v>596</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
@@ -6569,7 +6572,7 @@
         <v>1976</v>
       </c>
       <c r="B523" t="s">
-        <v>269</v>
+        <v>486</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
@@ -6577,7 +6580,7 @@
         <v>1976</v>
       </c>
       <c r="B524" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.25">
@@ -6585,15 +6588,15 @@
         <v>1976</v>
       </c>
       <c r="B525" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A526" s="1">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="B526" t="s">
-        <v>631</v>
+        <v>270</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.25">
@@ -6601,7 +6604,7 @@
         <v>1977</v>
       </c>
       <c r="B527" t="s">
-        <v>271</v>
+        <v>631</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
@@ -6609,7 +6612,7 @@
         <v>1977</v>
       </c>
       <c r="B528" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
@@ -6617,7 +6620,7 @@
         <v>1977</v>
       </c>
       <c r="B529" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.25">
@@ -6625,7 +6628,7 @@
         <v>1977</v>
       </c>
       <c r="B530" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.25">
@@ -6633,15 +6636,15 @@
         <v>1977</v>
       </c>
       <c r="B531" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A532" s="1">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="B532" t="s">
-        <v>487</v>
+        <v>276</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.25">
@@ -6649,15 +6652,15 @@
         <v>1978</v>
       </c>
       <c r="B533" t="s">
-        <v>277</v>
+        <v>487</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A534" s="1">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="B534" t="s">
-        <v>586</v>
+        <v>277</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.25">
@@ -6665,7 +6668,7 @@
         <v>1979</v>
       </c>
       <c r="B535" t="s">
-        <v>488</v>
+        <v>586</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
@@ -6673,15 +6676,15 @@
         <v>1979</v>
       </c>
       <c r="B536" t="s">
-        <v>278</v>
+        <v>488</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A537" s="1">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B537" t="s">
-        <v>490</v>
+        <v>278</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.25">
@@ -6689,7 +6692,7 @@
         <v>1980</v>
       </c>
       <c r="B538" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.25">
@@ -6697,7 +6700,7 @@
         <v>1980</v>
       </c>
       <c r="B539" t="s">
-        <v>284</v>
+        <v>489</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.25">
@@ -6705,15 +6708,15 @@
         <v>1980</v>
       </c>
       <c r="B540" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A541" s="1">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="B541" t="s">
-        <v>492</v>
+        <v>280</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.25">
@@ -6721,7 +6724,7 @@
         <v>1981</v>
       </c>
       <c r="B542" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.25">
@@ -6729,7 +6732,7 @@
         <v>1981</v>
       </c>
       <c r="B543" t="s">
-        <v>281</v>
+        <v>491</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.25">
@@ -6737,15 +6740,15 @@
         <v>1981</v>
       </c>
       <c r="B544" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A545" s="1">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="B545" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.25">
@@ -6753,7 +6756,7 @@
         <v>1982</v>
       </c>
       <c r="B546" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.25">
@@ -6761,7 +6764,7 @@
         <v>1982</v>
       </c>
       <c r="B547" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.25">
@@ -6769,15 +6772,15 @@
         <v>1982</v>
       </c>
       <c r="B548" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A549" s="1">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="B549" t="s">
-        <v>645</v>
+        <v>288</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.25">
@@ -6785,7 +6788,7 @@
         <v>1983</v>
       </c>
       <c r="B550" t="s">
-        <v>493</v>
+        <v>645</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.25">
@@ -6793,7 +6796,7 @@
         <v>1983</v>
       </c>
       <c r="B551" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.25">
@@ -6801,15 +6804,15 @@
         <v>1983</v>
       </c>
       <c r="B552" t="s">
-        <v>638</v>
+        <v>494</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A553" s="1">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="B553" t="s">
-        <v>496</v>
+        <v>638</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.25">
@@ -6817,7 +6820,7 @@
         <v>1984</v>
       </c>
       <c r="B554" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
@@ -6825,7 +6828,7 @@
         <v>1984</v>
       </c>
       <c r="B555" t="s">
-        <v>289</v>
+        <v>495</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.25">
@@ -6833,15 +6836,15 @@
         <v>1984</v>
       </c>
       <c r="B556" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A557" s="1">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="B557" t="s">
-        <v>626</v>
+        <v>290</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.25">
@@ -6849,7 +6852,7 @@
         <v>1985</v>
       </c>
       <c r="B558" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.25">
@@ -6857,15 +6860,15 @@
         <v>1985</v>
       </c>
       <c r="B559" t="s">
-        <v>291</v>
+        <v>627</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A560" s="1">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="B560" t="s">
-        <v>498</v>
+        <v>291</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.25">
@@ -6873,7 +6876,7 @@
         <v>1986</v>
       </c>
       <c r="B561" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.25">
@@ -6881,7 +6884,7 @@
         <v>1986</v>
       </c>
       <c r="B562" t="s">
-        <v>292</v>
+        <v>497</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.25">
@@ -6889,7 +6892,7 @@
         <v>1986</v>
       </c>
       <c r="B563" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.25">
@@ -6897,15 +6900,15 @@
         <v>1986</v>
       </c>
       <c r="B564" t="s">
-        <v>597</v>
+        <v>293</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A565" s="1">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="B565" t="s">
-        <v>499</v>
+        <v>597</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
@@ -6913,15 +6916,15 @@
         <v>1987</v>
       </c>
       <c r="B566" t="s">
-        <v>598</v>
+        <v>499</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A567" s="1">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="B567" t="s">
-        <v>294</v>
+        <v>598</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
@@ -6929,7 +6932,7 @@
         <v>1988</v>
       </c>
       <c r="B568" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.25">
@@ -6937,7 +6940,7 @@
         <v>1988</v>
       </c>
       <c r="B569" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.25">
@@ -6945,15 +6948,15 @@
         <v>1988</v>
       </c>
       <c r="B570" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A571" s="1">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="B571" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.25">
@@ -6961,7 +6964,7 @@
         <v>1989</v>
       </c>
       <c r="B572" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.25">
@@ -6969,15 +6972,15 @@
         <v>1989</v>
       </c>
       <c r="B573" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A574" s="1">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="B574" t="s">
-        <v>563</v>
+        <v>300</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.25">
@@ -6985,7 +6988,7 @@
         <v>1990</v>
       </c>
       <c r="B575" t="s">
-        <v>501</v>
+        <v>563</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.25">
@@ -6993,7 +6996,7 @@
         <v>1990</v>
       </c>
       <c r="B576" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.25">
@@ -7001,15 +7004,15 @@
         <v>1990</v>
       </c>
       <c r="B577" t="s">
-        <v>301</v>
+        <v>500</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A578" s="1">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="B578" t="s">
-        <v>502</v>
+        <v>301</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.25">
@@ -7017,7 +7020,7 @@
         <v>1991</v>
       </c>
       <c r="B579" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.25">
@@ -7025,15 +7028,15 @@
         <v>1991</v>
       </c>
       <c r="B580" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A581" s="1">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="B581" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.25">
@@ -7041,7 +7044,7 @@
         <v>1992</v>
       </c>
       <c r="B582" t="s">
-        <v>327</v>
+        <v>505</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.25">
@@ -7049,15 +7052,15 @@
         <v>1992</v>
       </c>
       <c r="B583" t="s">
-        <v>639</v>
+        <v>327</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A584" s="1">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="B584" t="s">
-        <v>506</v>
+        <v>639</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.25">
@@ -7065,15 +7068,15 @@
         <v>1993</v>
       </c>
       <c r="B585" t="s">
-        <v>326</v>
+        <v>506</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A586" s="1">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="B586" t="s">
-        <v>508</v>
+        <v>326</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.25">
@@ -7081,7 +7084,7 @@
         <v>1994</v>
       </c>
       <c r="B587" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.25">
@@ -7089,15 +7092,15 @@
         <v>1994</v>
       </c>
       <c r="B588" t="s">
-        <v>303</v>
+        <v>507</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A589" s="1">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B589" t="s">
-        <v>511</v>
+        <v>303</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.25">
@@ -7105,7 +7108,7 @@
         <v>1995</v>
       </c>
       <c r="B590" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.25">
@@ -7113,7 +7116,7 @@
         <v>1995</v>
       </c>
       <c r="B591" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.25">
@@ -7121,15 +7124,15 @@
         <v>1995</v>
       </c>
       <c r="B592" t="s">
-        <v>307</v>
+        <v>509</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A593" s="1">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="B593" t="s">
-        <v>512</v>
+        <v>307</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.25">
@@ -7137,15 +7140,15 @@
         <v>1996</v>
       </c>
       <c r="B594" t="s">
-        <v>310</v>
+        <v>512</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A595" s="1">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="B595" t="s">
-        <v>513</v>
+        <v>310</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.25">
@@ -7153,15 +7156,15 @@
         <v>1997</v>
       </c>
       <c r="B596" t="s">
-        <v>304</v>
+        <v>513</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A597" s="1">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B597" t="s">
-        <v>515</v>
+        <v>304</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.25">
@@ -7169,7 +7172,7 @@
         <v>1998</v>
       </c>
       <c r="B598" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.25">
@@ -7177,15 +7180,15 @@
         <v>1998</v>
       </c>
       <c r="B599" t="s">
-        <v>305</v>
+        <v>514</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A600" s="1">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B600" t="s">
-        <v>517</v>
+        <v>305</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.25">
@@ -7193,7 +7196,7 @@
         <v>1999</v>
       </c>
       <c r="B601" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.25">
@@ -7201,15 +7204,15 @@
         <v>1999</v>
       </c>
       <c r="B602" t="s">
-        <v>306</v>
+        <v>516</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A603" s="1">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="B603" t="s">
-        <v>518</v>
+        <v>306</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.25">
@@ -7217,7 +7220,7 @@
         <v>2000</v>
       </c>
       <c r="B604" t="s">
-        <v>311</v>
+        <v>518</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
@@ -7225,15 +7228,15 @@
         <v>2000</v>
       </c>
       <c r="B605" t="s">
-        <v>568</v>
+        <v>311</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A606" s="1">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B606" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.25">
@@ -7241,7 +7244,7 @@
         <v>2001</v>
       </c>
       <c r="B607" t="s">
-        <v>519</v>
+        <v>569</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.25">
@@ -7249,15 +7252,15 @@
         <v>2001</v>
       </c>
       <c r="B608" t="s">
-        <v>313</v>
+        <v>519</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A609" s="1">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B609" t="s">
-        <v>520</v>
+        <v>313</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.25">
@@ -7265,15 +7268,15 @@
         <v>2002</v>
       </c>
       <c r="B610" t="s">
-        <v>308</v>
+        <v>520</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A611" s="1">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B611" t="s">
-        <v>564</v>
+        <v>308</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.25">
@@ -7281,7 +7284,7 @@
         <v>2003</v>
       </c>
       <c r="B612" t="s">
-        <v>521</v>
+        <v>564</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
@@ -7289,15 +7292,15 @@
         <v>2003</v>
       </c>
       <c r="B613" t="s">
-        <v>312</v>
+        <v>521</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A614" s="1">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B614" t="s">
-        <v>570</v>
+        <v>312</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.25">
@@ -7305,7 +7308,7 @@
         <v>2004</v>
       </c>
       <c r="B615" t="s">
-        <v>522</v>
+        <v>570</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.25">
@@ -7313,7 +7316,7 @@
         <v>2004</v>
       </c>
       <c r="B616" t="s">
-        <v>571</v>
+        <v>522</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.25">
@@ -7321,15 +7324,15 @@
         <v>2004</v>
       </c>
       <c r="B617" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A618" s="1">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B618" t="s">
-        <v>523</v>
+        <v>580</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
@@ -7337,15 +7340,15 @@
         <v>2005</v>
       </c>
       <c r="B619" t="s">
-        <v>314</v>
+        <v>523</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A620" s="1">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B620" t="s">
-        <v>572</v>
+        <v>314</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.25">
@@ -7353,15 +7356,15 @@
         <v>2006</v>
       </c>
       <c r="B621" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A622" s="1">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B622" t="s">
-        <v>628</v>
+        <v>573</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
@@ -7369,15 +7372,15 @@
         <v>2007</v>
       </c>
       <c r="B623" t="s">
-        <v>315</v>
+        <v>628</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A624" s="1">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B624" t="s">
-        <v>524</v>
+        <v>315</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.25">
@@ -7385,15 +7388,15 @@
         <v>2008</v>
       </c>
       <c r="B625" t="s">
-        <v>630</v>
+        <v>524</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A626" s="1">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B626" t="s">
-        <v>525</v>
+        <v>630</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.25">
@@ -7401,15 +7404,15 @@
         <v>2009</v>
       </c>
       <c r="B627" t="s">
-        <v>316</v>
+        <v>525</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A628" s="1">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B628" t="s">
-        <v>526</v>
+        <v>316</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.25">
@@ -7417,15 +7420,15 @@
         <v>2010</v>
       </c>
       <c r="B629" t="s">
-        <v>317</v>
+        <v>526</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A630" s="1">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B630" t="s">
-        <v>565</v>
+        <v>317</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.25">
@@ -7433,7 +7436,7 @@
         <v>2011</v>
       </c>
       <c r="B631" t="s">
-        <v>527</v>
+        <v>565</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.25">
@@ -7441,15 +7444,15 @@
         <v>2011</v>
       </c>
       <c r="B632" t="s">
-        <v>318</v>
+        <v>527</v>
       </c>
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A633" s="1">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B633" t="s">
-        <v>574</v>
+        <v>318</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.25">
@@ -7457,15 +7460,15 @@
         <v>2012</v>
       </c>
       <c r="B634" t="s">
-        <v>319</v>
+        <v>574</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A635" s="1">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B635" t="s">
-        <v>528</v>
+        <v>319</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.25">
@@ -7473,15 +7476,15 @@
         <v>2013</v>
       </c>
       <c r="B636" t="s">
-        <v>320</v>
+        <v>528</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A637" s="1">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B637" t="s">
-        <v>529</v>
+        <v>320</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.25">
@@ -7489,7 +7492,7 @@
         <v>2014</v>
       </c>
       <c r="B638" t="s">
-        <v>629</v>
+        <v>529</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.25">
@@ -7497,15 +7500,15 @@
         <v>2014</v>
       </c>
       <c r="B639" t="s">
-        <v>640</v>
+        <v>629</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A640" s="1">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B640" t="s">
-        <v>530</v>
+        <v>640</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.25">
@@ -7513,15 +7516,15 @@
         <v>2015</v>
       </c>
       <c r="B641" t="s">
-        <v>321</v>
+        <v>530</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A642" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B642" t="s">
-        <v>532</v>
+        <v>321</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.25">
@@ -7529,7 +7532,7 @@
         <v>2016</v>
       </c>
       <c r="B643" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.25">
@@ -7537,15 +7540,15 @@
         <v>2016</v>
       </c>
       <c r="B644" t="s">
-        <v>322</v>
+        <v>531</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A645" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B645" t="s">
-        <v>567</v>
+        <v>322</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.25">
@@ -7553,7 +7556,7 @@
         <v>2017</v>
       </c>
       <c r="B646" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.25">
@@ -7561,7 +7564,7 @@
         <v>2017</v>
       </c>
       <c r="B647" t="s">
-        <v>323</v>
+        <v>566</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
@@ -7569,15 +7572,15 @@
         <v>2017</v>
       </c>
       <c r="B648" t="s">
-        <v>533</v>
+        <v>323</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A649" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B649" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.25">
@@ -7585,15 +7588,15 @@
         <v>2018</v>
       </c>
       <c r="B650" t="s">
-        <v>309</v>
+        <v>534</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A651" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B651" t="s">
-        <v>587</v>
+        <v>309</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.25">
@@ -7601,15 +7604,15 @@
         <v>2019</v>
       </c>
       <c r="B652" t="s">
-        <v>324</v>
+        <v>587</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A653" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B653" t="s">
-        <v>535</v>
+        <v>324</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.25">
@@ -7617,14 +7620,22 @@
         <v>2020</v>
       </c>
       <c r="B654" t="s">
-        <v>302</v>
+        <v>535</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A655" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B655" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="656" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A656" s="1">
         <v>2021</v>
       </c>
-      <c r="B655" t="s">
+      <c r="B656" t="s">
         <v>325</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Replaced some diacritics we missed with HTML entities, per review by David K.
</commit_message>
<xml_diff>
--- a/xlsx/historical_items.xlsx
+++ b/xlsx/historical_items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FAFB99-37DB-4238-BD25-9D362BDE89BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CA4B8E-35FD-4B59-B99A-154E6CFC1268}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{171EF181-1F3C-7A42-9B63-D835B687641B}"/>
   </bookViews>
@@ -1770,9 +1770,6 @@
     <t>First commercial high speed Maglev train starts operation between Shanghai and its airport.</t>
   </si>
   <si>
-    <t>The Oriental Railway Company opens the first section of railway in the Ottoman Empire, from İzmir to Seydiköy.</t>
-  </si>
-  <si>
     <t>Narrow gauge Catskill Mountain Railway opens to carry passengers from Hudson River steamboats to connections at Palenville, New York to the Catskill Mountain House destination resort.</t>
   </si>
   <si>
@@ -1878,9 +1875,6 @@
     <t>The first trains operate in what is now Romania between Oravi&amp;tcedil;a, Transylvania, and Bazia&amp;scedil;, on the Danube.</t>
   </si>
   <si>
-    <t>The Oriental Railway Company is granted the concession to build the first railway in Turkey, from &amp;Iuml;zmir to Aydın.</t>
-  </si>
-  <si>
     <t>New York line-Lenox-Becket-Sandisfield-Connecticut line Massachusetts Turnpike closes.</t>
   </si>
   <si>
@@ -1896,9 +1890,6 @@
     <t>Selandia launched - First ocean-going, diesel engine-driven ship.</t>
   </si>
   <si>
-    <t>The Luftkissengleitboot Hovercraft - First hovering vehicle was created by Dagobert Müller. It could only travel on water.</t>
-  </si>
-  <si>
     <t>The Turkestan-Siberia Railway is completed.</t>
   </si>
   <si>
@@ -1993,6 +1984,15 @@
   </si>
   <si>
     <t>The relocated northern portion of the MBTA Orange line opened to Sullivan in April, to Wellington in September, and to Malden in December.</t>
+  </si>
+  <si>
+    <t>The Oriental Railway Company is granted the concession to build the first railway in Turkey, from &amp;Iuml;zmir to Aydin.</t>
+  </si>
+  <si>
+    <t>The Luftkissengleitboot Hovercraft - First hovering vehicle was created by Dagobert M&amp;uuml;ller. It could only travel on water.</t>
+  </si>
+  <si>
+    <t>The Oriental Railway Company opens the first section of railway in the Ottoman Empire, from &amp;Iuml;zmir to Seydik&amp;ouml;y.</t>
   </si>
 </sst>
 </file>
@@ -2381,8 +2381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8479D0E-E3F6-DA41-AEC9-2CE4981D9A6E}">
   <dimension ref="A1:B656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A511" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B520" sqref="B520"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B185" sqref="B185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2393,10 +2393,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>599</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2412,7 +2412,7 @@
         <v>1800</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2420,7 +2420,7 @@
         <v>1800</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
         <v>1800</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2444,7 +2444,7 @@
         <v>1801</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3220,7 +3220,7 @@
         <v>1833</v>
       </c>
       <c r="B104" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -3244,7 +3244,7 @@
         <v>1834</v>
       </c>
       <c r="B107" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -3356,7 +3356,7 @@
         <v>1837</v>
       </c>
       <c r="B121" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -3364,7 +3364,7 @@
         <v>1837</v>
       </c>
       <c r="B122" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -3388,7 +3388,7 @@
         <v>1838</v>
       </c>
       <c r="B125" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -3524,7 +3524,7 @@
         <v>1844</v>
       </c>
       <c r="B142" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -3580,7 +3580,7 @@
         <v>1846</v>
       </c>
       <c r="B149" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -3596,7 +3596,7 @@
         <v>1846</v>
       </c>
       <c r="B151" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -3756,7 +3756,7 @@
         <v>1854</v>
       </c>
       <c r="B171" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -3772,7 +3772,7 @@
         <v>1854</v>
       </c>
       <c r="B173" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -3796,7 +3796,7 @@
         <v>1855</v>
       </c>
       <c r="B176" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -3828,7 +3828,7 @@
         <v>1856</v>
       </c>
       <c r="B180" t="s">
-        <v>617</v>
+        <v>653</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -3860,7 +3860,7 @@
         <v>1858</v>
       </c>
       <c r="B184" t="s">
-        <v>581</v>
+        <v>655</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -3892,7 +3892,7 @@
         <v>1859</v>
       </c>
       <c r="B188" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -3948,7 +3948,7 @@
         <v>1862</v>
       </c>
       <c r="B195" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -4076,7 +4076,7 @@
         <v>1870</v>
       </c>
       <c r="B211" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -4260,7 +4260,7 @@
         <v>1882</v>
       </c>
       <c r="B234" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -4476,7 +4476,7 @@
         <v>1893</v>
       </c>
       <c r="B261" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
@@ -4492,7 +4492,7 @@
         <v>1894</v>
       </c>
       <c r="B263" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
@@ -4500,7 +4500,7 @@
         <v>1894</v>
       </c>
       <c r="B264" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -4588,7 +4588,7 @@
         <v>1898</v>
       </c>
       <c r="B275" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
@@ -4604,7 +4604,7 @@
         <v>1899</v>
       </c>
       <c r="B277" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
@@ -4660,7 +4660,7 @@
         <v>1901</v>
       </c>
       <c r="B284" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
@@ -4700,7 +4700,7 @@
         <v>1903</v>
       </c>
       <c r="B289" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
@@ -4812,7 +4812,7 @@
         <v>1908</v>
       </c>
       <c r="B303" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
@@ -4908,7 +4908,7 @@
         <v>1911</v>
       </c>
       <c r="B315" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
@@ -4972,7 +4972,7 @@
         <v>1913</v>
       </c>
       <c r="B323" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
@@ -5020,7 +5020,7 @@
         <v>1915</v>
       </c>
       <c r="B329" t="s">
-        <v>623</v>
+        <v>654</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
@@ -5028,7 +5028,7 @@
         <v>1916</v>
       </c>
       <c r="B330" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
@@ -5060,7 +5060,7 @@
         <v>1917</v>
       </c>
       <c r="B334" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
@@ -5084,7 +5084,7 @@
         <v>1918</v>
       </c>
       <c r="B337" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
@@ -5132,7 +5132,7 @@
         <v>1921</v>
       </c>
       <c r="B343" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
@@ -5148,7 +5148,7 @@
         <v>1921</v>
       </c>
       <c r="B345" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
@@ -5172,7 +5172,7 @@
         <v>1923</v>
       </c>
       <c r="B348" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
@@ -5284,7 +5284,7 @@
         <v>1927</v>
       </c>
       <c r="B362" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
@@ -5340,7 +5340,7 @@
         <v>1930</v>
       </c>
       <c r="B369" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
@@ -5356,7 +5356,7 @@
         <v>1931</v>
       </c>
       <c r="B371" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
@@ -5372,7 +5372,7 @@
         <v>1932</v>
       </c>
       <c r="B373" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
@@ -5380,7 +5380,7 @@
         <v>1932</v>
       </c>
       <c r="B374" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
@@ -5916,7 +5916,7 @@
         <v>1955</v>
       </c>
       <c r="B441" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
@@ -5996,7 +5996,7 @@
         <v>1957</v>
       </c>
       <c r="B451" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
@@ -6140,7 +6140,7 @@
         <v>1962</v>
       </c>
       <c r="B469" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.25">
@@ -6164,7 +6164,7 @@
         <v>1962</v>
       </c>
       <c r="B472" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.25">
@@ -6172,7 +6172,7 @@
         <v>1962</v>
       </c>
       <c r="B473" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
@@ -6180,7 +6180,7 @@
         <v>1962</v>
       </c>
       <c r="B474" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.25">
@@ -6188,7 +6188,7 @@
         <v>1963</v>
       </c>
       <c r="B475" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
@@ -6196,7 +6196,7 @@
         <v>1963</v>
       </c>
       <c r="B476" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.25">
@@ -6284,7 +6284,7 @@
         <v>1966</v>
       </c>
       <c r="B487" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.25">
@@ -6356,7 +6356,7 @@
         <v>1967</v>
       </c>
       <c r="B496" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
@@ -6404,7 +6404,7 @@
         <v>1969</v>
       </c>
       <c r="B502" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
@@ -6428,7 +6428,7 @@
         <v>1969</v>
       </c>
       <c r="B505" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.25">
@@ -6444,7 +6444,7 @@
         <v>1970</v>
       </c>
       <c r="B507" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.25">
@@ -6476,7 +6476,7 @@
         <v>1972</v>
       </c>
       <c r="B511" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.25">
@@ -6540,7 +6540,7 @@
         <v>1975</v>
       </c>
       <c r="B519" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.25">
@@ -6564,7 +6564,7 @@
         <v>1975</v>
       </c>
       <c r="B522" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
@@ -6604,7 +6604,7 @@
         <v>1977</v>
       </c>
       <c r="B527" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.25">
@@ -6668,7 +6668,7 @@
         <v>1979</v>
       </c>
       <c r="B535" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.25">
@@ -6788,7 +6788,7 @@
         <v>1983</v>
       </c>
       <c r="B550" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.25">
@@ -6812,7 +6812,7 @@
         <v>1983</v>
       </c>
       <c r="B553" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.25">
@@ -6852,7 +6852,7 @@
         <v>1985</v>
       </c>
       <c r="B558" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.25">
@@ -6860,7 +6860,7 @@
         <v>1985</v>
       </c>
       <c r="B559" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.25">
@@ -6908,7 +6908,7 @@
         <v>1986</v>
       </c>
       <c r="B565" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
@@ -6924,7 +6924,7 @@
         <v>1987</v>
       </c>
       <c r="B567" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
@@ -7060,7 +7060,7 @@
         <v>1992</v>
       </c>
       <c r="B584" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.25">
@@ -7372,7 +7372,7 @@
         <v>2007</v>
       </c>
       <c r="B623" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
@@ -7396,7 +7396,7 @@
         <v>2008</v>
       </c>
       <c r="B626" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.25">
@@ -7500,7 +7500,7 @@
         <v>2014</v>
       </c>
       <c r="B639" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.25">
@@ -7508,7 +7508,7 @@
         <v>2014</v>
       </c>
       <c r="B640" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.25">
@@ -7604,7 +7604,7 @@
         <v>2019</v>
       </c>
       <c r="B652" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New spreadsheets from Ken: 07/01/2021.
</commit_message>
<xml_diff>
--- a/xlsx/historical_items.xlsx
+++ b/xlsx/historical_items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5296C2-E531-4056-9A1C-BEB09FD0DC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED7D3A1-BC20-4DF6-BD27-065AB06CDDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{171EF181-1F3C-7A42-9B63-D835B687641B}"/>
   </bookViews>
@@ -1581,9 +1581,6 @@
     <t>Opening of the Lynx Blue Line Extension in Charlotte, North Carolina.</t>
   </si>
   <si>
-    <t>Lund , Sweden tramway opened.</t>
-  </si>
-  <si>
     <t>Great Barrington and Alford Turnpike closes.</t>
   </si>
   <si>
@@ -1830,9 +1827,6 @@
     <t>The first section of the Paris Metro opens.</t>
   </si>
   <si>
-    <t>The first trains operate in what is now Romania between Oravița, Transylvania, and Baziaș, on the Danube.</t>
-  </si>
-  <si>
     <t>Long Island Railroad 401, the first diesel-electric locomotive used in mainline service, is demonstrated for the first time.</t>
   </si>
   <si>
@@ -1993,6 +1987,12 @@
   </si>
   <si>
     <t>Nantasket Beach Branch electrified. One of first U.S steam railroad electrifications.</t>
+  </si>
+  <si>
+    <t>The first trains operate in what is now Romania between Oravita, Transylvania, and Bazias, on the Danube.</t>
+  </si>
+  <si>
+    <t>Lund, Sweden tramway opened.</t>
   </si>
 </sst>
 </file>
@@ -2381,8 +2381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8479D0E-E3F6-DA41-AEC9-2CE4981D9A6E}">
   <dimension ref="A1:B656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A391" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A496" sqref="A496"/>
+    <sheetView tabSelected="1" topLeftCell="A630" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B654" sqref="B654"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2393,10 +2393,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>565</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2412,7 +2412,7 @@
         <v>1800</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2420,7 +2420,7 @@
         <v>1800</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
         <v>1800</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2436,7 +2436,7 @@
         <v>1800</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2444,7 +2444,7 @@
         <v>1801</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2484,7 +2484,7 @@
         <v>1803</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2508,7 +2508,7 @@
         <v>1803</v>
       </c>
       <c r="B15" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2532,7 +2532,7 @@
         <v>1804</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2540,7 +2540,7 @@
         <v>1804</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2564,7 +2564,7 @@
         <v>1805</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2572,7 +2572,7 @@
         <v>1806</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2580,7 +2580,7 @@
         <v>1805</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2596,7 +2596,7 @@
         <v>1806</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2700,7 +2700,7 @@
         <v>1811</v>
       </c>
       <c r="B39" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2740,7 +2740,7 @@
         <v>1812</v>
       </c>
       <c r="B44" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2828,7 +2828,7 @@
         <v>1834</v>
       </c>
       <c r="B55" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2892,7 +2892,7 @@
         <v>1821</v>
       </c>
       <c r="B63" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2908,7 +2908,7 @@
         <v>1822</v>
       </c>
       <c r="B65" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2916,7 +2916,7 @@
         <v>1803</v>
       </c>
       <c r="B66" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2940,7 +2940,7 @@
         <v>1824</v>
       </c>
       <c r="B69" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2996,7 +2996,7 @@
         <v>1827</v>
       </c>
       <c r="B76" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -3060,7 +3060,7 @@
         <v>1830</v>
       </c>
       <c r="B84" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -3100,7 +3100,7 @@
         <v>1830</v>
       </c>
       <c r="B89" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
         <v>1831</v>
       </c>
       <c r="B90" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -3188,7 +3188,7 @@
         <v>1833</v>
       </c>
       <c r="B100" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -3212,7 +3212,7 @@
         <v>1834</v>
       </c>
       <c r="B103" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -3268,7 +3268,7 @@
         <v>1836</v>
       </c>
       <c r="B110" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -3324,7 +3324,7 @@
         <v>1837</v>
       </c>
       <c r="B117" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -3332,7 +3332,7 @@
         <v>1837</v>
       </c>
       <c r="B118" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -3356,7 +3356,7 @@
         <v>1838</v>
       </c>
       <c r="B121" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -3428,7 +3428,7 @@
         <v>1841</v>
       </c>
       <c r="B130" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -3492,7 +3492,7 @@
         <v>1844</v>
       </c>
       <c r="B138" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -3540,7 +3540,7 @@
         <v>1846</v>
       </c>
       <c r="B144" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -3548,7 +3548,7 @@
         <v>1846</v>
       </c>
       <c r="B145" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -3564,7 +3564,7 @@
         <v>1846</v>
       </c>
       <c r="B147" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -3572,7 +3572,7 @@
         <v>1847</v>
       </c>
       <c r="B148" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -3596,7 +3596,7 @@
         <v>1848</v>
       </c>
       <c r="B151" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -3604,7 +3604,7 @@
         <v>1837</v>
       </c>
       <c r="B152" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -3612,7 +3612,7 @@
         <v>1848</v>
       </c>
       <c r="B153" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -3628,7 +3628,7 @@
         <v>1849</v>
       </c>
       <c r="B155" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -3652,7 +3652,7 @@
         <v>1850</v>
       </c>
       <c r="B158" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -3700,7 +3700,7 @@
         <v>1853</v>
       </c>
       <c r="B164" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -3716,7 +3716,7 @@
         <v>1854</v>
       </c>
       <c r="B166" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -3724,7 +3724,7 @@
         <v>1854</v>
       </c>
       <c r="B167" t="s">
-        <v>601</v>
+        <v>654</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -3740,7 +3740,7 @@
         <v>1854</v>
       </c>
       <c r="B169" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -3764,7 +3764,7 @@
         <v>1855</v>
       </c>
       <c r="B172" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -3796,7 +3796,7 @@
         <v>1856</v>
       </c>
       <c r="B176" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -3828,7 +3828,7 @@
         <v>1858</v>
       </c>
       <c r="B180" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -3860,7 +3860,7 @@
         <v>1859</v>
       </c>
       <c r="B184" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -3916,7 +3916,7 @@
         <v>1862</v>
       </c>
       <c r="B191" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -3956,7 +3956,7 @@
         <v>1865</v>
       </c>
       <c r="B196" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -3996,7 +3996,7 @@
         <v>1867</v>
       </c>
       <c r="B201" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -4004,7 +4004,7 @@
         <v>1867</v>
       </c>
       <c r="B202" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -4044,7 +4044,7 @@
         <v>1869</v>
       </c>
       <c r="B207" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -4060,7 +4060,7 @@
         <v>1870</v>
       </c>
       <c r="B209" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -4132,7 +4132,7 @@
         <v>1874</v>
       </c>
       <c r="B218" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
@@ -4148,7 +4148,7 @@
         <v>1875</v>
       </c>
       <c r="B220" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -4244,7 +4244,7 @@
         <v>1882</v>
       </c>
       <c r="B232" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -4276,7 +4276,7 @@
         <v>1883</v>
       </c>
       <c r="B236" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
@@ -4292,7 +4292,7 @@
         <v>1877</v>
       </c>
       <c r="B238" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -4332,7 +4332,7 @@
         <v>1887</v>
       </c>
       <c r="B243" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -4356,7 +4356,7 @@
         <v>1888</v>
       </c>
       <c r="B246" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -4372,7 +4372,7 @@
         <v>1888</v>
       </c>
       <c r="B248" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
@@ -4492,7 +4492,7 @@
         <v>1893</v>
       </c>
       <c r="B263" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
@@ -4508,7 +4508,7 @@
         <v>1894</v>
       </c>
       <c r="B265" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
@@ -4516,7 +4516,7 @@
         <v>1894</v>
       </c>
       <c r="B266" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
@@ -4524,7 +4524,7 @@
         <v>1893</v>
       </c>
       <c r="B267" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
@@ -4532,7 +4532,7 @@
         <v>1895</v>
       </c>
       <c r="B268" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
@@ -4540,7 +4540,7 @@
         <v>1895</v>
       </c>
       <c r="B269" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
@@ -4572,7 +4572,7 @@
         <v>1895</v>
       </c>
       <c r="B273" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
@@ -4628,7 +4628,7 @@
         <v>1898</v>
       </c>
       <c r="B280" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
@@ -4636,7 +4636,7 @@
         <v>1898</v>
       </c>
       <c r="B281" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
@@ -4644,7 +4644,7 @@
         <v>1899</v>
       </c>
       <c r="B282" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
@@ -4676,7 +4676,7 @@
         <v>1900</v>
       </c>
       <c r="B286" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
@@ -4684,7 +4684,7 @@
         <v>1900</v>
       </c>
       <c r="B287" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
@@ -4716,7 +4716,7 @@
         <v>1901</v>
       </c>
       <c r="B291" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
@@ -4756,7 +4756,7 @@
         <v>1903</v>
       </c>
       <c r="B296" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
@@ -4948,7 +4948,7 @@
         <v>1911</v>
       </c>
       <c r="B320" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
         <v>1911</v>
       </c>
       <c r="B321" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
@@ -5020,7 +5020,7 @@
         <v>1913</v>
       </c>
       <c r="B329" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
@@ -5068,7 +5068,7 @@
         <v>1915</v>
       </c>
       <c r="B335" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
@@ -5116,7 +5116,7 @@
         <v>1918</v>
       </c>
       <c r="B341" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
@@ -5172,7 +5172,7 @@
         <v>1921</v>
       </c>
       <c r="B348" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
@@ -5244,7 +5244,7 @@
         <v>1924</v>
       </c>
       <c r="B357" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
@@ -5300,7 +5300,7 @@
         <v>1927</v>
       </c>
       <c r="B364" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
@@ -5356,7 +5356,7 @@
         <v>1930</v>
       </c>
       <c r="B371" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
@@ -5364,7 +5364,7 @@
         <v>1931</v>
       </c>
       <c r="B372" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
@@ -5380,7 +5380,7 @@
         <v>1931</v>
       </c>
       <c r="B374" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
@@ -5780,7 +5780,7 @@
         <v>1948</v>
       </c>
       <c r="B424" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
@@ -5892,7 +5892,7 @@
         <v>1953</v>
       </c>
       <c r="B438" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
@@ -5924,7 +5924,7 @@
         <v>1955</v>
       </c>
       <c r="B442" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
@@ -6004,7 +6004,7 @@
         <v>1957</v>
       </c>
       <c r="B452" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
@@ -6164,7 +6164,7 @@
         <v>1962</v>
       </c>
       <c r="B472" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.25">
@@ -6172,7 +6172,7 @@
         <v>1962</v>
       </c>
       <c r="B473" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.25">
@@ -6180,7 +6180,7 @@
         <v>1962</v>
       </c>
       <c r="B474" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.25">
@@ -6188,7 +6188,7 @@
         <v>1963</v>
       </c>
       <c r="B475" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.25">
@@ -6276,7 +6276,7 @@
         <v>1966</v>
       </c>
       <c r="B486" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.25">
@@ -6348,7 +6348,7 @@
         <v>1967</v>
       </c>
       <c r="B495" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.25">
@@ -6356,7 +6356,7 @@
         <v>1968</v>
       </c>
       <c r="B496" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.25">
@@ -6364,7 +6364,7 @@
         <v>1968</v>
       </c>
       <c r="B497" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.25">
@@ -6404,7 +6404,7 @@
         <v>1969</v>
       </c>
       <c r="B502" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.25">
@@ -6412,7 +6412,7 @@
         <v>1969</v>
       </c>
       <c r="B503" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.25">
@@ -6436,7 +6436,7 @@
         <v>1969</v>
       </c>
       <c r="B506" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.25">
@@ -6452,7 +6452,7 @@
         <v>1970</v>
       </c>
       <c r="B508" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.25">
@@ -6484,7 +6484,7 @@
         <v>1972</v>
       </c>
       <c r="B512" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.25">
@@ -6564,7 +6564,7 @@
         <v>1975</v>
       </c>
       <c r="B522" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.25">
@@ -6572,7 +6572,7 @@
         <v>1976</v>
       </c>
       <c r="B523" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.25">
@@ -6612,7 +6612,7 @@
         <v>1977</v>
       </c>
       <c r="B528" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.25">
@@ -6676,7 +6676,7 @@
         <v>1979</v>
       </c>
       <c r="B536" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.25">
@@ -6812,7 +6812,7 @@
         <v>1983</v>
       </c>
       <c r="B553" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.25">
@@ -6852,7 +6852,7 @@
         <v>1985</v>
       </c>
       <c r="B558" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.25">
@@ -6860,7 +6860,7 @@
         <v>1985</v>
       </c>
       <c r="B559" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.25">
@@ -6908,7 +6908,7 @@
         <v>1986</v>
       </c>
       <c r="B565" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.25">
@@ -6924,7 +6924,7 @@
         <v>1987</v>
       </c>
       <c r="B567" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.25">
@@ -6940,7 +6940,7 @@
         <v>1988</v>
       </c>
       <c r="B569" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.25">
@@ -6988,7 +6988,7 @@
         <v>1990</v>
       </c>
       <c r="B575" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.25">
@@ -7060,7 +7060,7 @@
         <v>1992</v>
       </c>
       <c r="B584" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.25">
@@ -7092,7 +7092,7 @@
         <v>1994</v>
       </c>
       <c r="B588" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.25">
@@ -7236,7 +7236,7 @@
         <v>2000</v>
       </c>
       <c r="B606" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.25">
@@ -7244,7 +7244,7 @@
         <v>2001</v>
       </c>
       <c r="B607" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.25">
@@ -7284,7 +7284,7 @@
         <v>2003</v>
       </c>
       <c r="B612" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.25">
@@ -7308,7 +7308,7 @@
         <v>2004</v>
       </c>
       <c r="B615" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.25">
@@ -7324,7 +7324,7 @@
         <v>2004</v>
       </c>
       <c r="B617" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.25">
@@ -7332,7 +7332,7 @@
         <v>2004</v>
       </c>
       <c r="B618" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.25">
@@ -7356,7 +7356,7 @@
         <v>2006</v>
       </c>
       <c r="B621" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.25">
@@ -7364,7 +7364,7 @@
         <v>2006</v>
       </c>
       <c r="B622" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.25">
@@ -7372,7 +7372,7 @@
         <v>2007</v>
       </c>
       <c r="B623" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.25">
@@ -7396,7 +7396,7 @@
         <v>2008</v>
       </c>
       <c r="B626" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.25">
@@ -7436,7 +7436,7 @@
         <v>2011</v>
       </c>
       <c r="B631" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.25">
@@ -7460,7 +7460,7 @@
         <v>2012</v>
       </c>
       <c r="B634" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.25">
@@ -7500,7 +7500,7 @@
         <v>2014</v>
       </c>
       <c r="B639" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.25">
@@ -7508,7 +7508,7 @@
         <v>2014</v>
       </c>
       <c r="B640" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.25">
@@ -7556,7 +7556,7 @@
         <v>2017</v>
       </c>
       <c r="B646" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.25">
@@ -7564,7 +7564,7 @@
         <v>2017</v>
       </c>
       <c r="B647" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.25">
@@ -7604,7 +7604,7 @@
         <v>2019</v>
       </c>
       <c r="B652" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.25">
@@ -7620,7 +7620,7 @@
         <v>2020</v>
       </c>
       <c r="B654" t="s">
-        <v>518</v>
+        <v>655</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>